<commit_message>
Update Workflows and Tests
</commit_message>
<xml_diff>
--- a/Cmf.Custom.Tests/MasterData/Files/150-MasterData-AMSOsram.xlsx
+++ b/Cmf.Custom.Tests/MasterData/Files/150-MasterData-AMSOsram.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25330"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25427"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\CMF\projects\AMSOSRAM\Cmf.Custom.Tests\MasterData\Files\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\CMF\Projects\AMSOSRAM\Cmf.Custom.Tests\MasterData\Files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0C756F94-5700-4EBB-B9F9-F811671B5C7E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9F081D3E-B121-47CE-AD61-E1AF1998D30D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" firstSheet="19" activeTab="24" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" firstSheet="22" activeTab="24" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Index" sheetId="2" r:id="rId1"/>
@@ -66,7 +66,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1904" uniqueCount="855">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1936" uniqueCount="857">
   <si>
     <t>Tab Name</t>
   </si>
@@ -2703,6 +2703,12 @@
   </si>
   <si>
     <t>5FICP1.RFID</t>
+  </si>
+  <si>
+    <t>5FICP1-LP1</t>
+  </si>
+  <si>
+    <t>5FICP1-LP2</t>
   </si>
 </sst>
 </file>
@@ -3054,9 +3060,9 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -3070,7 +3076,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>4</v>
       </c>
@@ -3081,7 +3087,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>7</v>
       </c>
@@ -3092,7 +3098,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
         <v>9</v>
       </c>
@@ -3103,7 +3109,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
         <v>11</v>
       </c>
@@ -3114,7 +3120,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
         <v>13</v>
       </c>
@@ -3128,7 +3134,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
         <v>17</v>
       </c>
@@ -3142,7 +3148,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
         <v>20</v>
       </c>
@@ -3156,7 +3162,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
         <v>23</v>
       </c>
@@ -3170,7 +3176,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
         <v>26</v>
       </c>
@@ -3184,7 +3190,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
         <v>29</v>
       </c>
@@ -3198,7 +3204,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
         <v>32</v>
       </c>
@@ -3212,7 +3218,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A13" s="1" t="s">
         <v>35</v>
       </c>
@@ -3226,7 +3232,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A14" s="1" t="s">
         <v>38</v>
       </c>
@@ -3237,7 +3243,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A15" s="1" t="s">
         <v>40</v>
       </c>
@@ -3248,7 +3254,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A16" s="1" t="s">
         <v>42</v>
       </c>
@@ -3262,7 +3268,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A17" s="1" t="s">
         <v>45</v>
       </c>
@@ -3276,7 +3282,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A18" s="1" t="s">
         <v>48</v>
       </c>
@@ -3290,7 +3296,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A19" s="1" t="s">
         <v>52</v>
       </c>
@@ -3304,7 +3310,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A20" s="1" t="s">
         <v>55</v>
       </c>
@@ -3318,7 +3324,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A21" s="1" t="s">
         <v>58</v>
       </c>
@@ -3329,7 +3335,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A22" s="1" t="s">
         <v>60</v>
       </c>
@@ -3340,7 +3346,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A23" s="1" t="s">
         <v>62</v>
       </c>
@@ -3354,7 +3360,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A24" s="1" t="s">
         <v>64</v>
       </c>
@@ -3368,7 +3374,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A25" s="1" t="s">
         <v>67</v>
       </c>
@@ -3382,7 +3388,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A26" s="1" t="s">
         <v>70</v>
       </c>
@@ -3396,7 +3402,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A27" s="1" t="s">
         <v>73</v>
       </c>
@@ -3410,7 +3416,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A28" s="1" t="s">
         <v>76</v>
       </c>
@@ -3421,7 +3427,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A29" s="1" t="s">
         <v>78</v>
       </c>
@@ -3435,7 +3441,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A30" s="1" t="s">
         <v>81</v>
       </c>
@@ -3449,7 +3455,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A31" s="1" t="s">
         <v>84</v>
       </c>
@@ -3457,7 +3463,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A32" s="1" t="s">
         <v>85</v>
       </c>
@@ -3465,7 +3471,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A33" s="1" t="s">
         <v>86</v>
       </c>
@@ -3479,7 +3485,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A34" s="1" t="s">
         <v>89</v>
       </c>
@@ -3493,7 +3499,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A35" s="1" t="s">
         <v>92</v>
       </c>
@@ -3507,7 +3513,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A36" s="1" t="s">
         <v>95</v>
       </c>
@@ -3521,7 +3527,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A37" s="1" t="s">
         <v>98</v>
       </c>
@@ -3535,7 +3541,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A38" s="1" t="s">
         <v>101</v>
       </c>
@@ -3549,7 +3555,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A39" s="1" t="s">
         <v>105</v>
       </c>
@@ -3563,7 +3569,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A40" s="1" t="s">
         <v>108</v>
       </c>
@@ -3577,7 +3583,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A41" s="1" t="s">
         <v>110</v>
       </c>
@@ -3591,7 +3597,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A42" s="1" t="s">
         <v>113</v>
       </c>
@@ -3605,7 +3611,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A43" s="1" t="s">
         <v>116</v>
       </c>
@@ -3616,7 +3622,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A44" s="1" t="s">
         <v>118</v>
       </c>
@@ -3630,7 +3636,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A45" s="1" t="s">
         <v>121</v>
       </c>
@@ -3644,7 +3650,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A46" s="1" t="s">
         <v>124</v>
       </c>
@@ -3658,7 +3664,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A47" s="1" t="s">
         <v>127</v>
       </c>
@@ -3672,7 +3678,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A48" s="1" t="s">
         <v>130</v>
       </c>
@@ -3686,7 +3692,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A49" s="1" t="s">
         <v>133</v>
       </c>
@@ -3700,7 +3706,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A50" s="1" t="s">
         <v>136</v>
       </c>
@@ -3711,7 +3717,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A51" s="1" t="s">
         <v>138</v>
       </c>
@@ -3722,7 +3728,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A52" s="1" t="s">
         <v>140</v>
       </c>
@@ -3733,7 +3739,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A53" s="1" t="s">
         <v>142</v>
       </c>
@@ -3744,7 +3750,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A54" s="1" t="s">
         <v>144</v>
       </c>
@@ -3755,7 +3761,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A55" s="1" t="s">
         <v>146</v>
       </c>
@@ -3766,7 +3772,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="56" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A56" s="1" t="s">
         <v>148</v>
       </c>
@@ -3777,7 +3783,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="57" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A57" s="1" t="s">
         <v>151</v>
       </c>
@@ -3791,7 +3797,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="58" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A58" s="1" t="s">
         <v>154</v>
       </c>
@@ -3805,7 +3811,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="59" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A59" s="1" t="s">
         <v>157</v>
       </c>
@@ -3816,7 +3822,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="60" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A60" s="1" t="s">
         <v>159</v>
       </c>
@@ -3830,7 +3836,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="61" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A61" s="1" t="s">
         <v>162</v>
       </c>
@@ -3841,7 +3847,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="62" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A62" s="1" t="s">
         <v>164</v>
       </c>
@@ -3852,7 +3858,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="63" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A63" s="1" t="s">
         <v>166</v>
       </c>
@@ -3866,7 +3872,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="64" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A64" s="1" t="s">
         <v>169</v>
       </c>
@@ -3880,7 +3886,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="65" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A65" s="1" t="s">
         <v>172</v>
       </c>
@@ -3891,7 +3897,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="66" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A66" s="1" t="s">
         <v>174</v>
       </c>
@@ -3905,7 +3911,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="67" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A67" s="1" t="s">
         <v>177</v>
       </c>
@@ -3916,7 +3922,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="68" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A68" s="1" t="s">
         <v>179</v>
       </c>
@@ -3927,7 +3933,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="69" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A69" s="1" t="s">
         <v>181</v>
       </c>
@@ -3938,7 +3944,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="70" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A70" s="1" t="s">
         <v>183</v>
       </c>
@@ -3949,7 +3955,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="71" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A71" s="1" t="s">
         <v>185</v>
       </c>
@@ -3963,7 +3969,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="72" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A72" s="1" t="s">
         <v>188</v>
       </c>
@@ -3974,7 +3980,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="73" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A73" s="1" t="s">
         <v>190</v>
       </c>
@@ -3985,7 +3991,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="74" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A74" s="1" t="s">
         <v>193</v>
       </c>
@@ -3999,7 +4005,7 @@
         <v>195</v>
       </c>
     </row>
-    <row r="75" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A75" s="1" t="s">
         <v>196</v>
       </c>
@@ -4013,7 +4019,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="76" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A76" s="1" t="s">
         <v>199</v>
       </c>
@@ -4024,7 +4030,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="77" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A77" s="1" t="s">
         <v>201</v>
       </c>
@@ -4038,7 +4044,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="78" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A78" s="1" t="s">
         <v>204</v>
       </c>
@@ -4052,7 +4058,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="79" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A79" s="1" t="s">
         <v>207</v>
       </c>
@@ -4066,7 +4072,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="80" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A80" s="1" t="s">
         <v>210</v>
       </c>
@@ -4077,7 +4083,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="81" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A81" s="1" t="s">
         <v>212</v>
       </c>
@@ -4091,7 +4097,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="82" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A82" s="1" t="s">
         <v>215</v>
       </c>
@@ -4105,7 +4111,7 @@
         <v>217</v>
       </c>
     </row>
-    <row r="83" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A83" s="1" t="s">
         <v>218</v>
       </c>
@@ -4116,7 +4122,7 @@
         <v>217</v>
       </c>
     </row>
-    <row r="84" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A84" s="1" t="s">
         <v>220</v>
       </c>
@@ -4130,7 +4136,7 @@
         <v>222</v>
       </c>
     </row>
-    <row r="85" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A85" s="1" t="s">
         <v>223</v>
       </c>
@@ -4144,7 +4150,7 @@
         <v>225</v>
       </c>
     </row>
-    <row r="86" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A86" s="1" t="s">
         <v>226</v>
       </c>
@@ -4158,7 +4164,7 @@
         <v>228</v>
       </c>
     </row>
-    <row r="87" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A87" s="1" t="s">
         <v>229</v>
       </c>
@@ -4169,7 +4175,7 @@
         <v>228</v>
       </c>
     </row>
-    <row r="88" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A88" s="1" t="s">
         <v>231</v>
       </c>
@@ -4180,7 +4186,7 @@
         <v>228</v>
       </c>
     </row>
-    <row r="89" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A89" s="1" t="s">
         <v>233</v>
       </c>
@@ -4191,7 +4197,7 @@
         <v>228</v>
       </c>
     </row>
-    <row r="90" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A90" s="1" t="s">
         <v>235</v>
       </c>
@@ -4205,7 +4211,7 @@
         <v>237</v>
       </c>
     </row>
-    <row r="91" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A91" s="1" t="s">
         <v>238</v>
       </c>
@@ -4216,7 +4222,7 @@
         <v>237</v>
       </c>
     </row>
-    <row r="92" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A92" s="1" t="s">
         <v>240</v>
       </c>
@@ -4227,7 +4233,7 @@
         <v>237</v>
       </c>
     </row>
-    <row r="93" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A93" s="1" t="s">
         <v>242</v>
       </c>
@@ -4241,7 +4247,7 @@
         <v>244</v>
       </c>
     </row>
-    <row r="94" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A94" s="1" t="s">
         <v>245</v>
       </c>
@@ -4252,7 +4258,7 @@
         <v>244</v>
       </c>
     </row>
-    <row r="95" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A95" s="1" t="s">
         <v>247</v>
       </c>
@@ -4266,7 +4272,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="96" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A96" s="1" t="s">
         <v>251</v>
       </c>
@@ -4277,7 +4283,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="97" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A97" s="1" t="s">
         <v>253</v>
       </c>
@@ -4288,7 +4294,7 @@
         <v>254</v>
       </c>
     </row>
-    <row r="98" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A98" s="1" t="s">
         <v>255</v>
       </c>
@@ -4302,7 +4308,7 @@
         <v>258</v>
       </c>
     </row>
-    <row r="99" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A99" s="1" t="s">
         <v>259</v>
       </c>
@@ -4310,7 +4316,7 @@
         <v>258</v>
       </c>
     </row>
-    <row r="100" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A100" s="1" t="s">
         <v>260</v>
       </c>
@@ -4318,7 +4324,7 @@
         <v>258</v>
       </c>
     </row>
-    <row r="101" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A101" s="1" t="s">
         <v>261</v>
       </c>
@@ -4332,7 +4338,7 @@
         <v>263</v>
       </c>
     </row>
-    <row r="102" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A102" s="1" t="s">
         <v>264</v>
       </c>
@@ -4346,7 +4352,7 @@
         <v>266</v>
       </c>
     </row>
-    <row r="103" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A103" s="1" t="s">
         <v>267</v>
       </c>
@@ -4360,7 +4366,7 @@
         <v>269</v>
       </c>
     </row>
-    <row r="104" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A104" s="1" t="s">
         <v>270</v>
       </c>
@@ -4371,7 +4377,7 @@
         <v>269</v>
       </c>
     </row>
-    <row r="105" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A105" s="1" t="s">
         <v>272</v>
       </c>
@@ -4385,7 +4391,7 @@
         <v>274</v>
       </c>
     </row>
-    <row r="106" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A106" s="1" t="s">
         <v>275</v>
       </c>
@@ -4399,7 +4405,7 @@
         <v>277</v>
       </c>
     </row>
-    <row r="107" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A107" s="1" t="s">
         <v>278</v>
       </c>
@@ -4413,7 +4419,7 @@
         <v>280</v>
       </c>
     </row>
-    <row r="108" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A108" s="1" t="s">
         <v>281</v>
       </c>
@@ -4427,7 +4433,7 @@
         <v>283</v>
       </c>
     </row>
-    <row r="109" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A109" s="1" t="s">
         <v>284</v>
       </c>
@@ -4441,7 +4447,7 @@
         <v>286</v>
       </c>
     </row>
-    <row r="110" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A110" s="1" t="s">
         <v>287</v>
       </c>
@@ -4455,7 +4461,7 @@
         <v>289</v>
       </c>
     </row>
-    <row r="111" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A111" s="1" t="s">
         <v>290</v>
       </c>
@@ -4469,7 +4475,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="112" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A112" s="1" t="s">
         <v>293</v>
       </c>
@@ -4480,7 +4486,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="113" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A113" s="1" t="s">
         <v>295</v>
       </c>
@@ -4494,7 +4500,7 @@
         <v>297</v>
       </c>
     </row>
-    <row r="114" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A114" s="1" t="s">
         <v>298</v>
       </c>
@@ -4505,7 +4511,7 @@
         <v>297</v>
       </c>
     </row>
-    <row r="115" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A115" s="1" t="s">
         <v>300</v>
       </c>
@@ -4519,7 +4525,7 @@
         <v>302</v>
       </c>
     </row>
-    <row r="116" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A116" s="1" t="s">
         <v>303</v>
       </c>
@@ -4530,7 +4536,7 @@
         <v>302</v>
       </c>
     </row>
-    <row r="117" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A117" s="1" t="s">
         <v>305</v>
       </c>
@@ -4541,7 +4547,7 @@
         <v>302</v>
       </c>
     </row>
-    <row r="118" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A118" s="1" t="s">
         <v>307</v>
       </c>
@@ -4563,7 +4569,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData/>
   <pageMargins left="0.75" right="0.75" top="0.75" bottom="0.5" header="0.5" footer="0.75"/>
 </worksheet>
@@ -4575,7 +4581,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData/>
   <pageMargins left="0.75" right="0.75" top="0.75" bottom="0.5" header="0.5" footer="0.75"/>
 </worksheet>
@@ -4587,7 +4593,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData/>
   <pageMargins left="0.75" right="0.75" top="0.75" bottom="0.5" header="0.5" footer="0.75"/>
 </worksheet>
@@ -4599,7 +4605,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData/>
   <pageMargins left="0.75" right="0.75" top="0.75" bottom="0.5" header="0.5" footer="0.75"/>
 </worksheet>
@@ -4611,7 +4617,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData/>
   <pageMargins left="0.75" right="0.75" top="0.75" bottom="0.5" header="0.5" footer="0.75"/>
 </worksheet>
@@ -4623,9 +4629,9 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>617</v>
       </c>
@@ -4648,7 +4654,7 @@
         <v>623</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>624</v>
       </c>
@@ -4668,7 +4674,7 @@
         <v>534</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>625</v>
       </c>
@@ -4688,7 +4694,7 @@
         <v>534</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
         <v>625</v>
       </c>
@@ -4708,7 +4714,7 @@
         <v>534</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
         <v>625</v>
       </c>
@@ -4728,7 +4734,7 @@
         <v>534</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
         <v>626</v>
       </c>
@@ -4759,9 +4765,9 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>549</v>
       </c>
@@ -4787,7 +4793,7 @@
         <v>631</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>632</v>
       </c>
@@ -4813,7 +4819,7 @@
         <v>609</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>635</v>
       </c>
@@ -4839,7 +4845,7 @@
         <v>609</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
         <v>637</v>
       </c>
@@ -4876,9 +4882,9 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>514</v>
       </c>
@@ -4904,7 +4910,7 @@
         <v>644</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>637</v>
       </c>
@@ -4915,7 +4921,7 @@
         <v>609</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>637</v>
       </c>
@@ -4929,7 +4935,7 @@
         <v>646</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
         <v>637</v>
       </c>
@@ -4940,7 +4946,7 @@
         <v>609</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
         <v>637</v>
       </c>
@@ -4951,7 +4957,7 @@
         <v>609</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
         <v>637</v>
       </c>
@@ -4962,7 +4968,7 @@
         <v>609</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
         <v>637</v>
       </c>
@@ -4973,7 +4979,7 @@
         <v>609</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
         <v>637</v>
       </c>
@@ -4984,7 +4990,7 @@
         <v>609</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
         <v>637</v>
       </c>
@@ -4995,7 +5001,7 @@
         <v>609</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
         <v>637</v>
       </c>
@@ -5006,7 +5012,7 @@
         <v>609</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
         <v>632</v>
       </c>
@@ -5017,7 +5023,7 @@
         <v>609</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
         <v>632</v>
       </c>
@@ -5028,7 +5034,7 @@
         <v>609</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A13" s="1" t="s">
         <v>635</v>
       </c>
@@ -5050,7 +5056,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData/>
   <pageMargins left="0.75" right="0.75" top="0.75" bottom="0.5" header="0.5" footer="0.75"/>
 </worksheet>
@@ -5058,82 +5064,82 @@
 
 <file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1200-000000000000}">
-  <dimension ref="A1:BN12"/>
+  <dimension ref="A1:BN14"/>
   <sheetViews>
-    <sheetView topLeftCell="A8" workbookViewId="0">
-      <selection activeCell="A12" sqref="A11:A12"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A13" sqref="A13:A14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="13.28515625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="37.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="7.7109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="13.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="37.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="7.6640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.88671875" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="17" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="7.5703125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="7.5546875" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="7" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="13.5703125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="13.42578125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="7.5703125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="11.42578125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="14.28515625" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="12.5703125" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="28.140625" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="14.85546875" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="13.42578125" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="8.28515625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="13.5546875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="13.44140625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="7.5546875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="11.44140625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="14.33203125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="12.5546875" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="28.109375" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="14.88671875" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="13.44140625" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="8.33203125" bestFit="1" customWidth="1"/>
     <col min="18" max="18" width="32" bestFit="1" customWidth="1"/>
     <col min="19" max="19" width="19" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="16.85546875" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="11.42578125" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="30.140625" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="16.88671875" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="11.44140625" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="30.109375" bestFit="1" customWidth="1"/>
     <col min="23" max="23" width="25" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="24.7109375" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="36.85546875" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="20.28515625" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="27.85546875" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="22.28515625" bestFit="1" customWidth="1"/>
-    <col min="29" max="29" width="13.28515625" bestFit="1" customWidth="1"/>
-    <col min="30" max="30" width="16.42578125" bestFit="1" customWidth="1"/>
-    <col min="31" max="31" width="24.5703125" bestFit="1" customWidth="1"/>
-    <col min="32" max="32" width="13.5703125" bestFit="1" customWidth="1"/>
-    <col min="33" max="33" width="9.7109375" bestFit="1" customWidth="1"/>
-    <col min="34" max="34" width="12.140625" bestFit="1" customWidth="1"/>
-    <col min="35" max="35" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="24.6640625" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="36.88671875" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="20.33203125" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="27.88671875" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="22.33203125" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="13.33203125" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="16.44140625" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="24.5546875" bestFit="1" customWidth="1"/>
+    <col min="32" max="32" width="13.5546875" bestFit="1" customWidth="1"/>
+    <col min="33" max="33" width="9.6640625" bestFit="1" customWidth="1"/>
+    <col min="34" max="34" width="12.109375" bestFit="1" customWidth="1"/>
+    <col min="35" max="35" width="11.5546875" bestFit="1" customWidth="1"/>
     <col min="36" max="36" width="29" bestFit="1" customWidth="1"/>
-    <col min="37" max="37" width="28.85546875" bestFit="1" customWidth="1"/>
-    <col min="38" max="38" width="20.5703125" bestFit="1" customWidth="1"/>
-    <col min="39" max="39" width="17.42578125" bestFit="1" customWidth="1"/>
-    <col min="40" max="40" width="26.7109375" bestFit="1" customWidth="1"/>
-    <col min="41" max="41" width="21.42578125" bestFit="1" customWidth="1"/>
-    <col min="42" max="42" width="9.5703125" bestFit="1" customWidth="1"/>
-    <col min="43" max="43" width="27.7109375" bestFit="1" customWidth="1"/>
-    <col min="44" max="44" width="10.140625" bestFit="1" customWidth="1"/>
-    <col min="45" max="45" width="15.140625" bestFit="1" customWidth="1"/>
-    <col min="46" max="46" width="8.42578125" bestFit="1" customWidth="1"/>
-    <col min="47" max="47" width="36.7109375" bestFit="1" customWidth="1"/>
-    <col min="48" max="48" width="14.7109375" bestFit="1" customWidth="1"/>
-    <col min="49" max="49" width="13.5703125" bestFit="1" customWidth="1"/>
-    <col min="50" max="50" width="14.28515625" bestFit="1" customWidth="1"/>
+    <col min="37" max="37" width="28.88671875" bestFit="1" customWidth="1"/>
+    <col min="38" max="38" width="20.5546875" bestFit="1" customWidth="1"/>
+    <col min="39" max="39" width="17.44140625" bestFit="1" customWidth="1"/>
+    <col min="40" max="40" width="26.6640625" bestFit="1" customWidth="1"/>
+    <col min="41" max="41" width="21.44140625" bestFit="1" customWidth="1"/>
+    <col min="42" max="42" width="9.5546875" bestFit="1" customWidth="1"/>
+    <col min="43" max="43" width="27.6640625" bestFit="1" customWidth="1"/>
+    <col min="44" max="44" width="10.109375" bestFit="1" customWidth="1"/>
+    <col min="45" max="45" width="15.109375" bestFit="1" customWidth="1"/>
+    <col min="46" max="46" width="8.44140625" bestFit="1" customWidth="1"/>
+    <col min="47" max="47" width="36.6640625" bestFit="1" customWidth="1"/>
+    <col min="48" max="48" width="14.6640625" bestFit="1" customWidth="1"/>
+    <col min="49" max="49" width="13.5546875" bestFit="1" customWidth="1"/>
+    <col min="50" max="50" width="14.33203125" bestFit="1" customWidth="1"/>
     <col min="51" max="51" width="31" bestFit="1" customWidth="1"/>
-    <col min="52" max="52" width="30.42578125" bestFit="1" customWidth="1"/>
-    <col min="53" max="53" width="48.28515625" bestFit="1" customWidth="1"/>
+    <col min="52" max="52" width="30.44140625" bestFit="1" customWidth="1"/>
+    <col min="53" max="53" width="48.33203125" bestFit="1" customWidth="1"/>
     <col min="54" max="54" width="16" bestFit="1" customWidth="1"/>
     <col min="55" max="55" width="21" bestFit="1" customWidth="1"/>
-    <col min="56" max="56" width="15.28515625" bestFit="1" customWidth="1"/>
-    <col min="57" max="57" width="22.140625" bestFit="1" customWidth="1"/>
-    <col min="58" max="59" width="16.28515625" bestFit="1" customWidth="1"/>
-    <col min="60" max="60" width="18.5703125" bestFit="1" customWidth="1"/>
-    <col min="61" max="61" width="24.7109375" bestFit="1" customWidth="1"/>
-    <col min="62" max="62" width="20.85546875" bestFit="1" customWidth="1"/>
-    <col min="63" max="63" width="12.7109375" bestFit="1" customWidth="1"/>
-    <col min="64" max="64" width="15.42578125" bestFit="1" customWidth="1"/>
-    <col min="65" max="65" width="15.28515625" bestFit="1" customWidth="1"/>
+    <col min="56" max="56" width="15.33203125" bestFit="1" customWidth="1"/>
+    <col min="57" max="57" width="22.109375" bestFit="1" customWidth="1"/>
+    <col min="58" max="59" width="16.33203125" bestFit="1" customWidth="1"/>
+    <col min="60" max="60" width="18.5546875" bestFit="1" customWidth="1"/>
+    <col min="61" max="61" width="24.6640625" bestFit="1" customWidth="1"/>
+    <col min="62" max="62" width="20.88671875" bestFit="1" customWidth="1"/>
+    <col min="63" max="63" width="12.6640625" bestFit="1" customWidth="1"/>
+    <col min="64" max="64" width="15.44140625" bestFit="1" customWidth="1"/>
+    <col min="65" max="65" width="15.33203125" bestFit="1" customWidth="1"/>
     <col min="66" max="66" width="25" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:66" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:66" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>549</v>
       </c>
@@ -5333,7 +5339,7 @@
         <v>699</v>
       </c>
     </row>
-    <row r="2" spans="1:66" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:66" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>700</v>
       </c>
@@ -5377,7 +5383,7 @@
         <v>452</v>
       </c>
     </row>
-    <row r="3" spans="1:66" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:66" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>706</v>
       </c>
@@ -5424,7 +5430,7 @@
         <v>498</v>
       </c>
     </row>
-    <row r="4" spans="1:66" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:66" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
         <v>709</v>
       </c>
@@ -5471,7 +5477,7 @@
         <v>498</v>
       </c>
     </row>
-    <row r="5" spans="1:66" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:66" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
         <v>711</v>
       </c>
@@ -5518,7 +5524,7 @@
         <v>498</v>
       </c>
     </row>
-    <row r="6" spans="1:66" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:66" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
         <v>713</v>
       </c>
@@ -5565,7 +5571,7 @@
         <v>498</v>
       </c>
     </row>
-    <row r="7" spans="1:66" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:66" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
         <v>715</v>
       </c>
@@ -5609,7 +5615,7 @@
         <v>452</v>
       </c>
     </row>
-    <row r="8" spans="1:66" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:66" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
         <v>717</v>
       </c>
@@ -5653,7 +5659,7 @@
         <v>452</v>
       </c>
     </row>
-    <row r="9" spans="1:66" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:66" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
         <v>719</v>
       </c>
@@ -5697,7 +5703,7 @@
         <v>452</v>
       </c>
     </row>
-    <row r="10" spans="1:66" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:66" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
         <v>721</v>
       </c>
@@ -5741,7 +5747,7 @@
         <v>452</v>
       </c>
     </row>
-    <row r="11" spans="1:66" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:66" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>849</v>
       </c>
@@ -5785,7 +5791,7 @@
         <v>452</v>
       </c>
     </row>
-    <row r="12" spans="1:66" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:66" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>854</v>
       </c>
@@ -5826,6 +5832,94 @@
         <v>534</v>
       </c>
       <c r="AD12" s="1" t="s">
+        <v>452</v>
+      </c>
+    </row>
+    <row r="13" spans="1:66" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
+        <v>855</v>
+      </c>
+      <c r="B13" t="s">
+        <v>850</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>411</v>
+      </c>
+      <c r="D13" s="1" t="s">
+        <v>609</v>
+      </c>
+      <c r="E13" s="1" t="s">
+        <v>702</v>
+      </c>
+      <c r="F13" s="1" t="s">
+        <v>851</v>
+      </c>
+      <c r="G13" s="1" t="s">
+        <v>703</v>
+      </c>
+      <c r="L13" s="1" t="s">
+        <v>704</v>
+      </c>
+      <c r="M13" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="N13" s="1" t="s">
+        <v>609</v>
+      </c>
+      <c r="O13" s="1" t="s">
+        <v>413</v>
+      </c>
+      <c r="V13" s="1" t="s">
+        <v>534</v>
+      </c>
+      <c r="Z13" s="1" t="s">
+        <v>534</v>
+      </c>
+      <c r="AD13" s="1" t="s">
+        <v>452</v>
+      </c>
+    </row>
+    <row r="14" spans="1:66" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
+        <v>856</v>
+      </c>
+      <c r="B14" t="s">
+        <v>850</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>411</v>
+      </c>
+      <c r="D14" s="1" t="s">
+        <v>609</v>
+      </c>
+      <c r="E14" s="1" t="s">
+        <v>702</v>
+      </c>
+      <c r="F14" s="1" t="s">
+        <v>851</v>
+      </c>
+      <c r="G14" s="1" t="s">
+        <v>703</v>
+      </c>
+      <c r="L14" s="1" t="s">
+        <v>704</v>
+      </c>
+      <c r="M14" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="N14" s="1" t="s">
+        <v>609</v>
+      </c>
+      <c r="O14" s="1" t="s">
+        <v>413</v>
+      </c>
+      <c r="V14" s="1" t="s">
+        <v>534</v>
+      </c>
+      <c r="Z14" s="1" t="s">
+        <v>534</v>
+      </c>
+      <c r="AD14" s="1" t="s">
         <v>452</v>
       </c>
     </row>
@@ -5841,9 +5935,9 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>309</v>
       </c>
@@ -5857,7 +5951,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>312</v>
       </c>
@@ -5871,7 +5965,7 @@
         <v>315</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>312</v>
       </c>
@@ -5885,7 +5979,7 @@
         <v>318</v>
       </c>
     </row>
-    <row r="4" spans="1:4" ht="409.5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" ht="388.8" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
         <v>312</v>
       </c>
@@ -5899,7 +5993,7 @@
         <v>321</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
         <v>38</v>
       </c>
@@ -5913,7 +6007,7 @@
         <v>324</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
         <v>40</v>
       </c>
@@ -5927,7 +6021,7 @@
         <v>324</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
         <v>76</v>
       </c>
@@ -5941,7 +6035,7 @@
         <v>328</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
         <v>329</v>
       </c>
@@ -5955,7 +6049,7 @@
         <v>332</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
         <v>162</v>
       </c>
@@ -5969,7 +6063,7 @@
         <v>335</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
         <v>336</v>
       </c>
@@ -5983,7 +6077,7 @@
         <v>339</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
         <v>336</v>
       </c>
@@ -5997,7 +6091,7 @@
         <v>342</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
         <v>336</v>
       </c>
@@ -6011,7 +6105,7 @@
         <v>345</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A13" s="1" t="s">
         <v>346</v>
       </c>
@@ -6025,7 +6119,7 @@
         <v>349</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A14" s="1" t="s">
         <v>199</v>
       </c>
@@ -6039,7 +6133,7 @@
         <v>351</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A15" s="1" t="s">
         <v>352</v>
       </c>
@@ -6053,7 +6147,7 @@
         <v>355</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A16" s="1" t="s">
         <v>218</v>
       </c>
@@ -6067,7 +6161,7 @@
         <v>358</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A17" s="1" t="s">
         <v>359</v>
       </c>
@@ -6081,7 +6175,7 @@
         <v>361</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A18" s="1" t="s">
         <v>359</v>
       </c>
@@ -6095,7 +6189,7 @@
         <v>364</v>
       </c>
     </row>
-    <row r="19" spans="1:4" ht="405" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:4" ht="360" x14ac:dyDescent="0.3">
       <c r="A19" s="1" t="s">
         <v>231</v>
       </c>
@@ -6120,7 +6214,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData/>
   <pageMargins left="0.75" right="0.75" top="0.75" bottom="0.5" header="0.5" footer="0.75"/>
 </worksheet>
@@ -6132,7 +6226,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData/>
   <pageMargins left="0.75" right="0.75" top="0.75" bottom="0.5" header="0.5" footer="0.75"/>
 </worksheet>
@@ -6144,7 +6238,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData/>
   <pageMargins left="0.75" right="0.75" top="0.75" bottom="0.5" header="0.5" footer="0.75"/>
 </worksheet>
@@ -6154,9 +6248,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1600-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="M28" sqref="M28"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData/>
   <pageMargins left="0.75" right="0.75" top="0.75" bottom="0.5" header="0.5" footer="0.75"/>
 </worksheet>
@@ -6168,7 +6264,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData/>
   <pageMargins left="0.75" right="0.75" top="0.75" bottom="0.5" header="0.5" footer="0.75"/>
 </worksheet>
@@ -6176,15 +6272,18 @@
 
 <file path=xl/worksheets/sheet25.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1800-000000000000}">
-  <dimension ref="A1:C10"/>
+  <dimension ref="A1:C12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+      <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="2" max="2" width="12.44140625" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>617</v>
       </c>
@@ -6195,7 +6294,7 @@
         <v>723</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>700</v>
       </c>
@@ -6203,7 +6302,7 @@
         <v>706</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>700</v>
       </c>
@@ -6211,7 +6310,7 @@
         <v>709</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
         <v>700</v>
       </c>
@@ -6219,7 +6318,7 @@
         <v>711</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
         <v>700</v>
       </c>
@@ -6227,7 +6326,7 @@
         <v>713</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
         <v>700</v>
       </c>
@@ -6235,7 +6334,7 @@
         <v>715</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
         <v>700</v>
       </c>
@@ -6243,7 +6342,7 @@
         <v>717</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
         <v>700</v>
       </c>
@@ -6251,7 +6350,7 @@
         <v>719</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
         <v>700</v>
       </c>
@@ -6259,12 +6358,28 @@
         <v>721</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>849</v>
       </c>
       <c r="B10" t="s">
         <v>854</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>849</v>
+      </c>
+      <c r="B11" t="s">
+        <v>855</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
+        <v>849</v>
+      </c>
+      <c r="B12" t="s">
+        <v>856</v>
       </c>
     </row>
   </sheetData>
@@ -6278,9 +6393,9 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>617</v>
       </c>
@@ -6291,7 +6406,7 @@
         <v>629</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>700</v>
       </c>
@@ -6313,7 +6428,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData/>
   <pageMargins left="0.75" right="0.75" top="0.75" bottom="0.5" header="0.5" footer="0.75"/>
 </worksheet>
@@ -6325,7 +6440,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData/>
   <pageMargins left="0.75" right="0.75" top="0.75" bottom="0.5" header="0.5" footer="0.75"/>
 </worksheet>
@@ -6337,7 +6452,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData/>
   <pageMargins left="0.75" right="0.75" top="0.75" bottom="0.5" header="0.5" footer="0.75"/>
 </worksheet>
@@ -6349,9 +6464,9 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>309</v>
       </c>
@@ -6359,7 +6474,7 @@
         <v>368</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>312</v>
       </c>
@@ -6367,7 +6482,7 @@
         <v>369</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>312</v>
       </c>
@@ -6375,7 +6490,7 @@
         <v>370</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
         <v>330</v>
       </c>
@@ -6383,7 +6498,7 @@
         <v>371</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
         <v>372</v>
       </c>
@@ -6391,7 +6506,7 @@
         <v>373</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
         <v>374</v>
       </c>
@@ -6410,7 +6525,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData/>
   <pageMargins left="0.75" right="0.75" top="0.75" bottom="0.5" header="0.5" footer="0.75"/>
 </worksheet>
@@ -6422,7 +6537,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData/>
   <pageMargins left="0.75" right="0.75" top="0.75" bottom="0.5" header="0.5" footer="0.75"/>
 </worksheet>
@@ -6434,7 +6549,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData/>
   <pageMargins left="0.75" right="0.75" top="0.75" bottom="0.5" header="0.5" footer="0.75"/>
 </worksheet>
@@ -6446,7 +6561,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData/>
   <pageMargins left="0.75" right="0.75" top="0.75" bottom="0.5" header="0.5" footer="0.75"/>
 </worksheet>
@@ -6458,7 +6573,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData/>
   <pageMargins left="0.75" right="0.75" top="0.75" bottom="0.5" header="0.5" footer="0.75"/>
 </worksheet>
@@ -6470,7 +6585,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData/>
   <pageMargins left="0.75" right="0.75" top="0.75" bottom="0.5" header="0.5" footer="0.75"/>
 </worksheet>
@@ -6482,7 +6597,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData/>
   <pageMargins left="0.75" right="0.75" top="0.75" bottom="0.5" header="0.5" footer="0.75"/>
 </worksheet>
@@ -6494,7 +6609,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData/>
   <pageMargins left="0.75" right="0.75" top="0.75" bottom="0.5" header="0.5" footer="0.75"/>
 </worksheet>
@@ -6506,7 +6621,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData/>
   <pageMargins left="0.75" right="0.75" top="0.75" bottom="0.5" header="0.5" footer="0.75"/>
 </worksheet>
@@ -6518,9 +6633,9 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>549</v>
       </c>
@@ -6543,7 +6658,7 @@
         <v>728</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>729</v>
       </c>
@@ -6560,7 +6675,7 @@
         <v>731</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>732</v>
       </c>
@@ -6577,7 +6692,7 @@
         <v>731</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
         <v>733</v>
       </c>
@@ -6594,7 +6709,7 @@
         <v>731</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
         <v>734</v>
       </c>
@@ -6611,7 +6726,7 @@
         <v>731</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
         <v>735</v>
       </c>
@@ -6628,7 +6743,7 @@
         <v>731</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
         <v>736</v>
       </c>
@@ -6645,7 +6760,7 @@
         <v>731</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
         <v>737</v>
       </c>
@@ -6662,7 +6777,7 @@
         <v>731</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
         <v>738</v>
       </c>
@@ -6679,7 +6794,7 @@
         <v>731</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
         <v>739</v>
       </c>
@@ -6696,7 +6811,7 @@
         <v>731</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
         <v>740</v>
       </c>
@@ -6713,7 +6828,7 @@
         <v>731</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
         <v>741</v>
       </c>
@@ -6730,7 +6845,7 @@
         <v>731</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A13" s="1" t="s">
         <v>742</v>
       </c>
@@ -6747,7 +6862,7 @@
         <v>731</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A14" s="1" t="s">
         <v>743</v>
       </c>
@@ -6775,9 +6890,9 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>375</v>
       </c>
@@ -6785,7 +6900,7 @@
         <v>376</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>377</v>
       </c>
@@ -6793,7 +6908,7 @@
         <v>378</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>293</v>
       </c>
@@ -6801,7 +6916,7 @@
         <v>379</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
         <v>140</v>
       </c>
@@ -6809,7 +6924,7 @@
         <v>380</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
         <v>142</v>
       </c>
@@ -6828,9 +6943,9 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>744</v>
       </c>
@@ -6874,7 +6989,7 @@
         <v>752</v>
       </c>
     </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>729</v>
       </c>
@@ -6897,7 +7012,7 @@
         <v>754</v>
       </c>
     </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>729</v>
       </c>
@@ -6920,7 +7035,7 @@
         <v>754</v>
       </c>
     </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
         <v>729</v>
       </c>
@@ -6943,7 +7058,7 @@
         <v>754</v>
       </c>
     </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
         <v>740</v>
       </c>
@@ -6960,7 +7075,7 @@
         <v>754</v>
       </c>
     </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
         <v>740</v>
       </c>
@@ -6977,7 +7092,7 @@
         <v>754</v>
       </c>
     </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
         <v>740</v>
       </c>
@@ -6994,7 +7109,7 @@
         <v>754</v>
       </c>
     </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
         <v>740</v>
       </c>
@@ -7011,7 +7126,7 @@
         <v>754</v>
       </c>
     </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
         <v>732</v>
       </c>
@@ -7034,7 +7149,7 @@
         <v>754</v>
       </c>
     </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
         <v>732</v>
       </c>
@@ -7057,7 +7172,7 @@
         <v>754</v>
       </c>
     </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
         <v>763</v>
       </c>
@@ -7077,7 +7192,7 @@
         <v>754</v>
       </c>
     </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
         <v>733</v>
       </c>
@@ -7100,7 +7215,7 @@
         <v>754</v>
       </c>
     </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A13" s="1" t="s">
         <v>733</v>
       </c>
@@ -7123,7 +7238,7 @@
         <v>754</v>
       </c>
     </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A14" s="1" t="s">
         <v>733</v>
       </c>
@@ -7146,7 +7261,7 @@
         <v>754</v>
       </c>
     </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A15" s="1" t="s">
         <v>733</v>
       </c>
@@ -7169,7 +7284,7 @@
         <v>754</v>
       </c>
     </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A16" s="1" t="s">
         <v>733</v>
       </c>
@@ -7192,7 +7307,7 @@
         <v>754</v>
       </c>
     </row>
-    <row r="17" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A17" s="1" t="s">
         <v>741</v>
       </c>
@@ -7209,7 +7324,7 @@
         <v>754</v>
       </c>
     </row>
-    <row r="18" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A18" s="1" t="s">
         <v>741</v>
       </c>
@@ -7226,7 +7341,7 @@
         <v>754</v>
       </c>
     </row>
-    <row r="19" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A19" s="1" t="s">
         <v>741</v>
       </c>
@@ -7243,7 +7358,7 @@
         <v>754</v>
       </c>
     </row>
-    <row r="20" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A20" s="1" t="s">
         <v>773</v>
       </c>
@@ -7263,7 +7378,7 @@
         <v>754</v>
       </c>
     </row>
-    <row r="21" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A21" s="1" t="s">
         <v>734</v>
       </c>
@@ -7286,7 +7401,7 @@
         <v>754</v>
       </c>
     </row>
-    <row r="22" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A22" s="1" t="s">
         <v>742</v>
       </c>
@@ -7303,7 +7418,7 @@
         <v>754</v>
       </c>
     </row>
-    <row r="23" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A23" s="1" t="s">
         <v>777</v>
       </c>
@@ -7323,7 +7438,7 @@
         <v>754</v>
       </c>
     </row>
-    <row r="24" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A24" s="1" t="s">
         <v>735</v>
       </c>
@@ -7346,7 +7461,7 @@
         <v>754</v>
       </c>
     </row>
-    <row r="25" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A25" s="1" t="s">
         <v>735</v>
       </c>
@@ -7369,7 +7484,7 @@
         <v>754</v>
       </c>
     </row>
-    <row r="26" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A26" s="1" t="s">
         <v>735</v>
       </c>
@@ -7392,7 +7507,7 @@
         <v>754</v>
       </c>
     </row>
-    <row r="27" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A27" s="1" t="s">
         <v>735</v>
       </c>
@@ -7415,7 +7530,7 @@
         <v>754</v>
       </c>
     </row>
-    <row r="28" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A28" s="1" t="s">
         <v>735</v>
       </c>
@@ -7438,7 +7553,7 @@
         <v>754</v>
       </c>
     </row>
-    <row r="29" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A29" s="1" t="s">
         <v>743</v>
       </c>
@@ -7455,7 +7570,7 @@
         <v>754</v>
       </c>
     </row>
-    <row r="30" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A30" s="1" t="s">
         <v>785</v>
       </c>
@@ -7475,7 +7590,7 @@
         <v>754</v>
       </c>
     </row>
-    <row r="31" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A31" s="1" t="s">
         <v>736</v>
       </c>
@@ -7498,7 +7613,7 @@
         <v>754</v>
       </c>
     </row>
-    <row r="32" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A32" s="1" t="s">
         <v>736</v>
       </c>
@@ -7521,7 +7636,7 @@
         <v>754</v>
       </c>
     </row>
-    <row r="33" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A33" s="1" t="s">
         <v>736</v>
       </c>
@@ -7544,7 +7659,7 @@
         <v>754</v>
       </c>
     </row>
-    <row r="34" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A34" s="1" t="s">
         <v>736</v>
       </c>
@@ -7567,7 +7682,7 @@
         <v>754</v>
       </c>
     </row>
-    <row r="35" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A35" s="1" t="s">
         <v>736</v>
       </c>
@@ -7590,7 +7705,7 @@
         <v>754</v>
       </c>
     </row>
-    <row r="36" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A36" s="1" t="s">
         <v>737</v>
       </c>
@@ -7613,7 +7728,7 @@
         <v>754</v>
       </c>
     </row>
-    <row r="37" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A37" s="1" t="s">
         <v>737</v>
       </c>
@@ -7636,7 +7751,7 @@
         <v>754</v>
       </c>
     </row>
-    <row r="38" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A38" s="1" t="s">
         <v>738</v>
       </c>
@@ -7659,7 +7774,7 @@
         <v>754</v>
       </c>
     </row>
-    <row r="39" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A39" s="1" t="s">
         <v>738</v>
       </c>
@@ -7682,7 +7797,7 @@
         <v>754</v>
       </c>
     </row>
-    <row r="40" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A40" s="1" t="s">
         <v>738</v>
       </c>
@@ -7705,7 +7820,7 @@
         <v>754</v>
       </c>
     </row>
-    <row r="41" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A41" s="1" t="s">
         <v>738</v>
       </c>
@@ -7728,7 +7843,7 @@
         <v>754</v>
       </c>
     </row>
-    <row r="42" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A42" s="1" t="s">
         <v>739</v>
       </c>
@@ -7751,7 +7866,7 @@
         <v>754</v>
       </c>
     </row>
-    <row r="43" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A43" s="1" t="s">
         <v>739</v>
       </c>
@@ -7774,7 +7889,7 @@
         <v>754</v>
       </c>
     </row>
-    <row r="44" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A44" s="1" t="s">
         <v>739</v>
       </c>
@@ -7797,7 +7912,7 @@
         <v>754</v>
       </c>
     </row>
-    <row r="45" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A45" s="1" t="s">
         <v>739</v>
       </c>
@@ -7831,7 +7946,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData/>
   <pageMargins left="0.75" right="0.75" top="0.75" bottom="0.5" header="0.5" footer="0.75"/>
 </worksheet>
@@ -7843,7 +7958,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData/>
   <pageMargins left="0.75" right="0.75" top="0.75" bottom="0.5" header="0.5" footer="0.75"/>
 </worksheet>
@@ -7855,9 +7970,9 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>549</v>
       </c>
@@ -7904,7 +8019,7 @@
         <v>811</v>
       </c>
     </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>812</v>
       </c>
@@ -7948,7 +8063,7 @@
         <v>609</v>
       </c>
     </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>814</v>
       </c>
@@ -8003,9 +8118,9 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>816</v>
       </c>
@@ -8043,7 +8158,7 @@
         <v>824</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>812</v>
       </c>
@@ -8075,7 +8190,7 @@
         <v>450</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>812</v>
       </c>
@@ -8107,7 +8222,7 @@
         <v>449</v>
       </c>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
         <v>812</v>
       </c>
@@ -8139,7 +8254,7 @@
         <v>827</v>
       </c>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
         <v>812</v>
       </c>
@@ -8174,7 +8289,7 @@
         <v>829</v>
       </c>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
         <v>812</v>
       </c>
@@ -8209,7 +8324,7 @@
         <v>450</v>
       </c>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
         <v>812</v>
       </c>
@@ -8244,7 +8359,7 @@
         <v>450</v>
       </c>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
         <v>812</v>
       </c>
@@ -8276,7 +8391,7 @@
         <v>450</v>
       </c>
     </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
         <v>812</v>
       </c>
@@ -8308,7 +8423,7 @@
         <v>450</v>
       </c>
     </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
         <v>812</v>
       </c>
@@ -8340,7 +8455,7 @@
         <v>450</v>
       </c>
     </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
         <v>814</v>
       </c>
@@ -8372,7 +8487,7 @@
         <v>450</v>
       </c>
     </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
         <v>814</v>
       </c>
@@ -8404,7 +8519,7 @@
         <v>827</v>
       </c>
     </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A13" s="1" t="s">
         <v>814</v>
       </c>
@@ -8436,7 +8551,7 @@
         <v>829</v>
       </c>
     </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A14" s="1" t="s">
         <v>814</v>
       </c>
@@ -8479,9 +8594,9 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>549</v>
       </c>
@@ -8495,7 +8610,7 @@
         <v>832</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>813</v>
       </c>
@@ -8506,7 +8621,7 @@
         <v>834</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>815</v>
       </c>
@@ -8528,9 +8643,9 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>802</v>
       </c>
@@ -8553,7 +8668,7 @@
         <v>319</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>813</v>
       </c>
@@ -8570,7 +8685,7 @@
         <v>609</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>813</v>
       </c>
@@ -8587,7 +8702,7 @@
         <v>609</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
         <v>813</v>
       </c>
@@ -8604,7 +8719,7 @@
         <v>609</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
         <v>813</v>
       </c>
@@ -8621,7 +8736,7 @@
         <v>609</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
         <v>813</v>
       </c>
@@ -8638,7 +8753,7 @@
         <v>609</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
         <v>813</v>
       </c>
@@ -8655,7 +8770,7 @@
         <v>609</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
         <v>813</v>
       </c>
@@ -8672,7 +8787,7 @@
         <v>609</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
         <v>813</v>
       </c>
@@ -8689,7 +8804,7 @@
         <v>609</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
         <v>813</v>
       </c>
@@ -8706,7 +8821,7 @@
         <v>534</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
         <v>815</v>
       </c>
@@ -8723,7 +8838,7 @@
         <v>609</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
         <v>815</v>
       </c>
@@ -8740,7 +8855,7 @@
         <v>609</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A13" s="1" t="s">
         <v>815</v>
       </c>
@@ -8757,7 +8872,7 @@
         <v>609</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A14" s="1" t="s">
         <v>815</v>
       </c>
@@ -8785,9 +8900,9 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>802</v>
       </c>
@@ -8813,7 +8928,7 @@
         <v>840</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>813</v>
       </c>
@@ -8830,7 +8945,7 @@
         <v>732</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>813</v>
       </c>
@@ -8847,7 +8962,7 @@
         <v>733</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
         <v>813</v>
       </c>
@@ -8864,7 +8979,7 @@
         <v>734</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
         <v>813</v>
       </c>
@@ -8881,7 +8996,7 @@
         <v>735</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
         <v>813</v>
       </c>
@@ -8898,7 +9013,7 @@
         <v>736</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
         <v>813</v>
       </c>
@@ -8915,7 +9030,7 @@
         <v>737</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
         <v>813</v>
       </c>
@@ -8932,7 +9047,7 @@
         <v>738</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
         <v>813</v>
       </c>
@@ -8949,7 +9064,7 @@
         <v>739</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
         <v>815</v>
       </c>
@@ -8966,7 +9081,7 @@
         <v>741</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
         <v>815</v>
       </c>
@@ -8983,7 +9098,7 @@
         <v>742</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
         <v>815</v>
       </c>
@@ -9011,814 +9126,814 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>382</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>383</v>
       </c>
     </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>384</v>
       </c>
     </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
         <v>385</v>
       </c>
     </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
         <v>386</v>
       </c>
     </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
         <v>387</v>
       </c>
     </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
         <v>388</v>
       </c>
     </row>
-    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
         <v>389</v>
       </c>
     </row>
-    <row r="9" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
         <v>390</v>
       </c>
     </row>
-    <row r="10" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
         <v>391</v>
       </c>
     </row>
-    <row r="11" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
         <v>392</v>
       </c>
     </row>
-    <row r="12" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
         <v>393</v>
       </c>
     </row>
-    <row r="14" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>394</v>
       </c>
     </row>
-    <row r="15" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A15" s="1" t="s">
         <v>395</v>
       </c>
     </row>
-    <row r="16" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A16" s="1" t="s">
         <v>396</v>
       </c>
     </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A17" s="1" t="s">
         <v>397</v>
       </c>
     </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>398</v>
       </c>
     </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A20" s="1" t="s">
         <v>399</v>
       </c>
     </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A21" s="1" t="s">
         <v>400</v>
       </c>
     </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>401</v>
       </c>
     </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A24" s="1" t="s">
         <v>402</v>
       </c>
     </row>
-    <row r="25" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A25" s="1" t="s">
         <v>403</v>
       </c>
     </row>
-    <row r="26" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A26" s="1" t="s">
         <v>404</v>
       </c>
     </row>
-    <row r="27" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A27" s="1" t="s">
         <v>405</v>
       </c>
     </row>
-    <row r="29" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
         <v>406</v>
       </c>
     </row>
-    <row r="30" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A30" s="1" t="s">
         <v>407</v>
       </c>
     </row>
-    <row r="31" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A31" s="1" t="s">
         <v>408</v>
       </c>
     </row>
-    <row r="32" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A32" s="1" t="s">
         <v>409</v>
       </c>
     </row>
-    <row r="34" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
         <v>410</v>
       </c>
     </row>
-    <row r="35" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A35" s="1" t="s">
         <v>411</v>
       </c>
     </row>
-    <row r="36" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A36" s="1" t="s">
         <v>412</v>
       </c>
     </row>
-    <row r="37" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A37" s="1" t="s">
         <v>413</v>
       </c>
     </row>
-    <row r="38" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A38" s="1" t="s">
         <v>414</v>
       </c>
     </row>
-    <row r="39" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A39" s="1" t="s">
         <v>415</v>
       </c>
     </row>
-    <row r="40" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A40" s="1" t="s">
         <v>416</v>
       </c>
     </row>
-    <row r="41" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A41" s="1" t="s">
         <v>417</v>
       </c>
     </row>
-    <row r="42" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A42" s="1" t="s">
         <v>418</v>
       </c>
     </row>
-    <row r="44" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
         <v>419</v>
       </c>
     </row>
-    <row r="45" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A45" s="1" t="s">
         <v>420</v>
       </c>
     </row>
-    <row r="46" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A46" s="1" t="s">
         <v>421</v>
       </c>
     </row>
-    <row r="47" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A47" s="1" t="s">
         <v>422</v>
       </c>
     </row>
-    <row r="48" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A48" s="1" t="s">
         <v>423</v>
       </c>
     </row>
-    <row r="50" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
         <v>424</v>
       </c>
     </row>
-    <row r="51" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A51" s="1" t="s">
         <v>425</v>
       </c>
     </row>
-    <row r="52" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A52" s="1" t="s">
         <v>426</v>
       </c>
     </row>
-    <row r="54" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A54" t="s">
         <v>427</v>
       </c>
     </row>
-    <row r="55" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A55" s="1" t="s">
         <v>428</v>
       </c>
     </row>
-    <row r="56" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A56" s="1" t="s">
         <v>429</v>
       </c>
     </row>
-    <row r="57" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A57" s="1" t="s">
         <v>430</v>
       </c>
     </row>
-    <row r="58" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A58" s="1" t="s">
         <v>431</v>
       </c>
     </row>
-    <row r="59" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A59" s="1" t="s">
         <v>432</v>
       </c>
     </row>
-    <row r="60" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A60" s="1" t="s">
         <v>433</v>
       </c>
     </row>
-    <row r="61" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A61" s="1" t="s">
         <v>434</v>
       </c>
     </row>
-    <row r="62" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A62" s="1" t="s">
         <v>435</v>
       </c>
     </row>
-    <row r="64" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A64" t="s">
         <v>436</v>
       </c>
     </row>
-    <row r="65" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A65" s="1" t="s">
         <v>437</v>
       </c>
     </row>
-    <row r="66" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A66" s="1" t="s">
         <v>438</v>
       </c>
     </row>
-    <row r="68" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A68" t="s">
         <v>439</v>
       </c>
     </row>
-    <row r="69" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A69" s="1" t="s">
         <v>440</v>
       </c>
     </row>
-    <row r="70" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A70" s="1" t="s">
         <v>441</v>
       </c>
     </row>
-    <row r="71" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A71" s="1" t="s">
         <v>442</v>
       </c>
     </row>
-    <row r="73" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A73" t="s">
         <v>443</v>
       </c>
     </row>
-    <row r="74" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A74" s="1" t="s">
         <v>444</v>
       </c>
     </row>
-    <row r="75" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A75" s="1" t="s">
         <v>445</v>
       </c>
     </row>
-    <row r="76" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A76" s="1" t="s">
         <v>446</v>
       </c>
     </row>
-    <row r="77" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A77" s="1" t="s">
         <v>447</v>
       </c>
     </row>
-    <row r="79" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A79" t="s">
         <v>448</v>
       </c>
     </row>
-    <row r="80" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A80" s="1" t="s">
         <v>449</v>
       </c>
     </row>
-    <row r="81" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A81" s="1" t="s">
         <v>450</v>
       </c>
     </row>
-    <row r="83" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A83" t="s">
         <v>451</v>
       </c>
     </row>
-    <row r="84" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A84" s="1" t="s">
         <v>450</v>
       </c>
     </row>
-    <row r="85" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A85" s="1" t="s">
         <v>452</v>
       </c>
     </row>
-    <row r="86" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A86" s="1" t="s">
         <v>403</v>
       </c>
     </row>
-    <row r="88" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A88" t="s">
         <v>453</v>
       </c>
     </row>
-    <row r="89" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A89" s="1" t="s">
         <v>454</v>
       </c>
     </row>
-    <row r="90" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A90" s="1" t="s">
         <v>455</v>
       </c>
     </row>
-    <row r="92" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A92" t="s">
         <v>456</v>
       </c>
     </row>
-    <row r="93" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A93" s="1" t="s">
         <v>457</v>
       </c>
     </row>
-    <row r="94" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A94" s="1" t="s">
         <v>458</v>
       </c>
     </row>
-    <row r="96" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A96" t="s">
         <v>459</v>
       </c>
     </row>
-    <row r="97" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A97" s="1" t="s">
         <v>460</v>
       </c>
     </row>
-    <row r="98" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A98" s="1" t="s">
         <v>461</v>
       </c>
     </row>
-    <row r="100" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A100" t="s">
         <v>462</v>
       </c>
     </row>
-    <row r="101" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A101" s="1" t="s">
         <v>463</v>
       </c>
     </row>
-    <row r="102" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A102" s="1" t="s">
         <v>464</v>
       </c>
     </row>
-    <row r="103" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A103" s="1" t="s">
         <v>465</v>
       </c>
     </row>
-    <row r="104" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A104" s="1" t="s">
         <v>466</v>
       </c>
     </row>
-    <row r="106" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A106" t="s">
         <v>467</v>
       </c>
     </row>
-    <row r="107" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A107" s="1" t="s">
         <v>468</v>
       </c>
     </row>
-    <row r="108" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A108" s="1" t="s">
         <v>469</v>
       </c>
     </row>
-    <row r="109" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A109" s="1" t="s">
         <v>470</v>
       </c>
     </row>
-    <row r="110" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A110" s="1" t="s">
         <v>471</v>
       </c>
     </row>
-    <row r="111" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A111" s="1" t="s">
         <v>472</v>
       </c>
     </row>
-    <row r="112" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A112" s="1" t="s">
         <v>473</v>
       </c>
     </row>
-    <row r="114" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A114" t="s">
         <v>474</v>
       </c>
     </row>
-    <row r="115" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A115" s="1" t="s">
         <v>475</v>
       </c>
     </row>
-    <row r="116" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A116" s="1" t="s">
         <v>476</v>
       </c>
     </row>
-    <row r="118" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A118" t="s">
         <v>477</v>
       </c>
     </row>
-    <row r="119" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A119" s="1" t="s">
         <v>464</v>
       </c>
     </row>
-    <row r="120" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A120" s="1" t="s">
         <v>463</v>
       </c>
     </row>
-    <row r="121" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A121" s="1" t="s">
         <v>478</v>
       </c>
     </row>
-    <row r="122" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A122" s="1" t="s">
         <v>479</v>
       </c>
     </row>
-    <row r="123" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A123" s="1" t="s">
         <v>480</v>
       </c>
     </row>
-    <row r="125" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A125" t="s">
         <v>481</v>
       </c>
     </row>
-    <row r="126" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A126" s="1" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="127" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A127" s="1" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="128" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A128" s="1" t="s">
         <v>482</v>
       </c>
     </row>
-    <row r="129" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A129" s="1" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="130" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A130" s="1" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="131" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A131" s="1" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="132" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A132" s="1" t="s">
         <v>483</v>
       </c>
     </row>
-    <row r="133" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A133" s="1" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="135" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A135" t="s">
         <v>484</v>
       </c>
     </row>
-    <row r="136" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A136" s="1" t="s">
         <v>485</v>
       </c>
     </row>
-    <row r="137" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A137" s="1" t="s">
         <v>486</v>
       </c>
     </row>
-    <row r="139" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A139" t="s">
         <v>487</v>
       </c>
     </row>
-    <row r="140" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A140" s="1" t="s">
         <v>488</v>
       </c>
     </row>
-    <row r="141" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A141" s="1" t="s">
         <v>489</v>
       </c>
     </row>
-    <row r="143" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="143" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A143" t="s">
         <v>490</v>
       </c>
     </row>
-    <row r="144" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="144" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A144" s="1" t="s">
         <v>491</v>
       </c>
     </row>
-    <row r="145" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="145" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A145" s="1" t="s">
         <v>449</v>
       </c>
     </row>
-    <row r="147" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="147" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A147" t="s">
         <v>492</v>
       </c>
     </row>
-    <row r="148" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="148" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A148" s="1" t="s">
         <v>493</v>
       </c>
     </row>
-    <row r="149" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="149" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A149" s="1" t="s">
         <v>494</v>
       </c>
     </row>
-    <row r="150" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="150" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A150" s="1" t="s">
         <v>495</v>
       </c>
     </row>
-    <row r="152" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="152" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A152" t="s">
         <v>496</v>
       </c>
     </row>
-    <row r="153" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="153" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A153" s="1" t="s">
         <v>497</v>
       </c>
     </row>
-    <row r="154" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="154" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A154" s="1" t="s">
         <v>498</v>
       </c>
     </row>
-    <row r="156" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="156" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A156" t="s">
         <v>499</v>
       </c>
     </row>
-    <row r="157" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="157" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A157" s="1" t="s">
         <v>500</v>
       </c>
     </row>
-    <row r="158" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="158" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A158" s="1" t="s">
         <v>501</v>
       </c>
     </row>
-    <row r="159" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="159" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A159" s="1" t="s">
         <v>502</v>
       </c>
     </row>
-    <row r="161" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="161" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A161" t="s">
         <v>503</v>
       </c>
     </row>
-    <row r="162" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="162" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A162" s="1" t="s">
         <v>504</v>
       </c>
     </row>
-    <row r="163" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="163" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A163" s="1" t="s">
         <v>505</v>
       </c>
     </row>
-    <row r="165" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="165" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A165" t="s">
         <v>506</v>
       </c>
     </row>
-    <row r="166" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="166" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A166" s="1" t="s">
         <v>507</v>
       </c>
     </row>
-    <row r="167" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="167" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A167" s="1" t="s">
         <v>508</v>
       </c>
     </row>
-    <row r="168" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="168" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A168" s="1" t="s">
         <v>509</v>
       </c>
     </row>
-    <row r="169" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="169" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A169" s="1" t="s">
         <v>510</v>
       </c>
     </row>
-    <row r="170" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="170" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A170" s="1" t="s">
         <v>415</v>
       </c>
     </row>
-    <row r="172" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="172" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A172" t="s">
         <v>511</v>
       </c>
     </row>
-    <row r="173" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="173" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A173" s="1" t="s">
         <v>468</v>
       </c>
     </row>
-    <row r="174" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="174" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A174" s="1" t="s">
         <v>403</v>
       </c>
     </row>
-    <row r="175" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="175" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A175" s="1" t="s">
         <v>404</v>
       </c>
     </row>
-    <row r="176" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="176" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A176" s="1" t="s">
         <v>497</v>
       </c>
     </row>
-    <row r="177" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="177" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A177" s="1" t="s">
         <v>512</v>
       </c>
     </row>
-    <row r="178" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="178" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A178" s="1" t="s">
         <v>513</v>
       </c>
     </row>
-    <row r="179" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="179" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A179" s="1" t="s">
         <v>514</v>
       </c>
     </row>
-    <row r="181" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="181" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A181" t="s">
         <v>515</v>
       </c>
     </row>
-    <row r="182" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="182" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A182" s="1" t="s">
         <v>516</v>
       </c>
     </row>
-    <row r="183" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="183" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A183" s="1" t="s">
         <v>517</v>
       </c>
     </row>
-    <row r="184" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="184" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A184" s="1" t="s">
         <v>518</v>
       </c>
     </row>
-    <row r="185" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="185" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A185" s="1" t="s">
         <v>519</v>
       </c>
     </row>
-    <row r="186" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="186" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A186" s="1" t="s">
         <v>520</v>
       </c>
     </row>
-    <row r="187" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="187" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A187" s="1" t="s">
         <v>521</v>
       </c>
     </row>
-    <row r="188" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="188" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A188" s="1" t="s">
         <v>522</v>
       </c>
     </row>
-    <row r="189" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="189" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A189" s="1" t="s">
         <v>523</v>
       </c>
     </row>
-    <row r="190" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="190" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A190" s="1" t="s">
         <v>485</v>
       </c>
     </row>
-    <row r="191" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="191" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A191" s="1" t="s">
         <v>524</v>
       </c>
     </row>
-    <row r="192" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="192" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A192" s="1" t="s">
         <v>525</v>
       </c>
     </row>
-    <row r="193" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="193" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A193" s="1" t="s">
         <v>526</v>
       </c>
@@ -9834,9 +9949,9 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>527</v>
       </c>
@@ -9853,7 +9968,7 @@
         <v>531</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>532</v>
       </c>
@@ -9867,7 +9982,7 @@
         <v>534</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>532</v>
       </c>
@@ -9881,7 +9996,7 @@
         <v>534</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
         <v>532</v>
       </c>
@@ -9895,7 +10010,7 @@
         <v>534</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
         <v>532</v>
       </c>
@@ -9909,7 +10024,7 @@
         <v>534</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
         <v>532</v>
       </c>
@@ -9923,7 +10038,7 @@
         <v>534</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
         <v>532</v>
       </c>
@@ -9937,7 +10052,7 @@
         <v>534</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
         <v>540</v>
       </c>
@@ -9951,7 +10066,7 @@
         <v>534</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
         <v>542</v>
       </c>
@@ -9965,7 +10080,7 @@
         <v>534</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
         <v>542</v>
       </c>
@@ -9979,7 +10094,7 @@
         <v>534</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
         <v>542</v>
       </c>
@@ -9993,7 +10108,7 @@
         <v>534</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
         <v>542</v>
       </c>
@@ -10007,7 +10122,7 @@
         <v>534</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A13" s="1" t="s">
         <v>542</v>
       </c>
@@ -10021,7 +10136,7 @@
         <v>534</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A14" s="1" t="s">
         <v>542</v>
       </c>
@@ -10035,7 +10150,7 @@
         <v>534</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A15" s="1" t="s">
         <v>547</v>
       </c>
@@ -10060,9 +10175,9 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>549</v>
       </c>
@@ -10079,7 +10194,7 @@
         <v>552</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>553</v>
       </c>
@@ -10090,7 +10205,7 @@
         <v>555</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>556</v>
       </c>
@@ -10101,7 +10216,7 @@
         <v>555</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
         <v>557</v>
       </c>
@@ -10112,7 +10227,7 @@
         <v>555</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
         <v>558</v>
       </c>
@@ -10123,7 +10238,7 @@
         <v>555</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
         <v>560</v>
       </c>
@@ -10145,9 +10260,9 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:47" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>549</v>
       </c>
@@ -10290,7 +10405,7 @@
         <v>604</v>
       </c>
     </row>
-    <row r="2" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:47" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>605</v>
       </c>
@@ -10334,7 +10449,7 @@
         <v>611</v>
       </c>
     </row>
-    <row r="3" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:47" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>612</v>
       </c>
@@ -10389,7 +10504,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData/>
   <pageMargins left="0.75" right="0.75" top="0.75" bottom="0.5" header="0.5" footer="0.75"/>
 </worksheet>

</xml_diff>

<commit_message>
Added placeholder step for testing purpouses
</commit_message>
<xml_diff>
--- a/Cmf.Custom.Tests/MasterData/Files/150-MasterData-AMSOsram.xlsx
+++ b/Cmf.Custom.Tests/MasterData/Files/150-MasterData-AMSOsram.xlsx
@@ -5,12 +5,12 @@
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\CMF\Projects\AMSOSRAM\Cmf.Custom.Tests\MasterData\Files\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Gits\AMSOSRAM\Cmf.Custom.Tests\MasterData\Files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9F081D3E-B121-47CE-AD61-E1AF1998D30D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4D2F1858-9745-439C-B99F-93B3F596971B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" firstSheet="22" activeTab="24" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1905" yWindow="1905" windowWidth="21600" windowHeight="11235" firstSheet="25" activeTab="25" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Index" sheetId="2" r:id="rId1"/>
@@ -66,7 +66,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1936" uniqueCount="857">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1939" uniqueCount="858">
   <si>
     <t>Tab Name</t>
   </si>
@@ -2709,6 +2709,9 @@
   </si>
   <si>
     <t>5FICP1-LP2</t>
+  </si>
+  <si>
+    <t>CD-Measurement</t>
   </si>
 </sst>
 </file>
@@ -3060,9 +3063,9 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -3076,7 +3079,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>4</v>
       </c>
@@ -3087,7 +3090,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>7</v>
       </c>
@@ -3098,7 +3101,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>9</v>
       </c>
@@ -3109,7 +3112,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>11</v>
       </c>
@@ -3120,7 +3123,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>13</v>
       </c>
@@ -3134,7 +3137,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>17</v>
       </c>
@@ -3148,7 +3151,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>20</v>
       </c>
@@ -3162,7 +3165,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>23</v>
       </c>
@@ -3176,7 +3179,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>26</v>
       </c>
@@ -3190,7 +3193,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>29</v>
       </c>
@@ -3204,7 +3207,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>32</v>
       </c>
@@ -3218,7 +3221,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>35</v>
       </c>
@@ -3232,7 +3235,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
         <v>38</v>
       </c>
@@ -3243,7 +3246,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
         <v>40</v>
       </c>
@@ -3254,7 +3257,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
         <v>42</v>
       </c>
@@ -3268,7 +3271,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
         <v>45</v>
       </c>
@@ -3282,7 +3285,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
         <v>48</v>
       </c>
@@ -3296,7 +3299,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
         <v>52</v>
       </c>
@@ -3310,7 +3313,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
         <v>55</v>
       </c>
@@ -3324,7 +3327,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
         <v>58</v>
       </c>
@@ -3335,7 +3338,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
         <v>60</v>
       </c>
@@ -3346,7 +3349,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
         <v>62</v>
       </c>
@@ -3360,7 +3363,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
         <v>64</v>
       </c>
@@ -3374,7 +3377,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
         <v>67</v>
       </c>
@@ -3388,7 +3391,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
         <v>70</v>
       </c>
@@ -3402,7 +3405,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
         <v>73</v>
       </c>
@@ -3416,7 +3419,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
         <v>76</v>
       </c>
@@ -3427,7 +3430,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A29" s="1" t="s">
         <v>78</v>
       </c>
@@ -3441,7 +3444,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A30" s="1" t="s">
         <v>81</v>
       </c>
@@ -3455,7 +3458,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A31" s="1" t="s">
         <v>84</v>
       </c>
@@ -3463,7 +3466,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A32" s="1" t="s">
         <v>85</v>
       </c>
@@ -3471,7 +3474,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A33" s="1" t="s">
         <v>86</v>
       </c>
@@ -3485,7 +3488,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A34" s="1" t="s">
         <v>89</v>
       </c>
@@ -3499,7 +3502,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A35" s="1" t="s">
         <v>92</v>
       </c>
@@ -3513,7 +3516,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A36" s="1" t="s">
         <v>95</v>
       </c>
@@ -3527,7 +3530,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A37" s="1" t="s">
         <v>98</v>
       </c>
@@ -3541,7 +3544,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A38" s="1" t="s">
         <v>101</v>
       </c>
@@ -3555,7 +3558,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A39" s="1" t="s">
         <v>105</v>
       </c>
@@ -3569,7 +3572,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A40" s="1" t="s">
         <v>108</v>
       </c>
@@ -3583,7 +3586,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A41" s="1" t="s">
         <v>110</v>
       </c>
@@ -3597,7 +3600,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A42" s="1" t="s">
         <v>113</v>
       </c>
@@ -3611,7 +3614,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A43" s="1" t="s">
         <v>116</v>
       </c>
@@ -3622,7 +3625,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A44" s="1" t="s">
         <v>118</v>
       </c>
@@ -3636,7 +3639,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A45" s="1" t="s">
         <v>121</v>
       </c>
@@ -3650,7 +3653,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A46" s="1" t="s">
         <v>124</v>
       </c>
@@ -3664,7 +3667,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A47" s="1" t="s">
         <v>127</v>
       </c>
@@ -3678,7 +3681,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A48" s="1" t="s">
         <v>130</v>
       </c>
@@ -3692,7 +3695,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A49" s="1" t="s">
         <v>133</v>
       </c>
@@ -3706,7 +3709,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A50" s="1" t="s">
         <v>136</v>
       </c>
@@ -3717,7 +3720,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A51" s="1" t="s">
         <v>138</v>
       </c>
@@ -3728,7 +3731,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A52" s="1" t="s">
         <v>140</v>
       </c>
@@ -3739,7 +3742,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A53" s="1" t="s">
         <v>142</v>
       </c>
@@ -3750,7 +3753,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A54" s="1" t="s">
         <v>144</v>
       </c>
@@ -3761,7 +3764,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A55" s="1" t="s">
         <v>146</v>
       </c>
@@ -3772,7 +3775,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="56" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A56" s="1" t="s">
         <v>148</v>
       </c>
@@ -3783,7 +3786,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="57" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A57" s="1" t="s">
         <v>151</v>
       </c>
@@ -3797,7 +3800,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="58" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A58" s="1" t="s">
         <v>154</v>
       </c>
@@ -3811,7 +3814,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="59" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A59" s="1" t="s">
         <v>157</v>
       </c>
@@ -3822,7 +3825,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="60" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A60" s="1" t="s">
         <v>159</v>
       </c>
@@ -3836,7 +3839,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="61" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A61" s="1" t="s">
         <v>162</v>
       </c>
@@ -3847,7 +3850,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="62" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A62" s="1" t="s">
         <v>164</v>
       </c>
@@ -3858,7 +3861,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="63" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A63" s="1" t="s">
         <v>166</v>
       </c>
@@ -3872,7 +3875,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="64" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A64" s="1" t="s">
         <v>169</v>
       </c>
@@ -3886,7 +3889,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="65" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A65" s="1" t="s">
         <v>172</v>
       </c>
@@ -3897,7 +3900,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="66" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A66" s="1" t="s">
         <v>174</v>
       </c>
@@ -3911,7 +3914,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="67" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A67" s="1" t="s">
         <v>177</v>
       </c>
@@ -3922,7 +3925,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="68" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A68" s="1" t="s">
         <v>179</v>
       </c>
@@ -3933,7 +3936,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="69" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A69" s="1" t="s">
         <v>181</v>
       </c>
@@ -3944,7 +3947,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="70" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A70" s="1" t="s">
         <v>183</v>
       </c>
@@ -3955,7 +3958,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="71" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A71" s="1" t="s">
         <v>185</v>
       </c>
@@ -3969,7 +3972,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="72" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A72" s="1" t="s">
         <v>188</v>
       </c>
@@ -3980,7 +3983,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="73" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A73" s="1" t="s">
         <v>190</v>
       </c>
@@ -3991,7 +3994,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="74" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A74" s="1" t="s">
         <v>193</v>
       </c>
@@ -4005,7 +4008,7 @@
         <v>195</v>
       </c>
     </row>
-    <row r="75" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A75" s="1" t="s">
         <v>196</v>
       </c>
@@ -4019,7 +4022,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="76" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A76" s="1" t="s">
         <v>199</v>
       </c>
@@ -4030,7 +4033,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="77" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A77" s="1" t="s">
         <v>201</v>
       </c>
@@ -4044,7 +4047,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="78" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A78" s="1" t="s">
         <v>204</v>
       </c>
@@ -4058,7 +4061,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="79" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A79" s="1" t="s">
         <v>207</v>
       </c>
@@ -4072,7 +4075,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="80" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A80" s="1" t="s">
         <v>210</v>
       </c>
@@ -4083,7 +4086,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="81" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A81" s="1" t="s">
         <v>212</v>
       </c>
@@ -4097,7 +4100,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="82" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A82" s="1" t="s">
         <v>215</v>
       </c>
@@ -4111,7 +4114,7 @@
         <v>217</v>
       </c>
     </row>
-    <row r="83" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A83" s="1" t="s">
         <v>218</v>
       </c>
@@ -4122,7 +4125,7 @@
         <v>217</v>
       </c>
     </row>
-    <row r="84" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A84" s="1" t="s">
         <v>220</v>
       </c>
@@ -4136,7 +4139,7 @@
         <v>222</v>
       </c>
     </row>
-    <row r="85" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A85" s="1" t="s">
         <v>223</v>
       </c>
@@ -4150,7 +4153,7 @@
         <v>225</v>
       </c>
     </row>
-    <row r="86" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A86" s="1" t="s">
         <v>226</v>
       </c>
@@ -4164,7 +4167,7 @@
         <v>228</v>
       </c>
     </row>
-    <row r="87" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A87" s="1" t="s">
         <v>229</v>
       </c>
@@ -4175,7 +4178,7 @@
         <v>228</v>
       </c>
     </row>
-    <row r="88" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A88" s="1" t="s">
         <v>231</v>
       </c>
@@ -4186,7 +4189,7 @@
         <v>228</v>
       </c>
     </row>
-    <row r="89" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A89" s="1" t="s">
         <v>233</v>
       </c>
@@ -4197,7 +4200,7 @@
         <v>228</v>
       </c>
     </row>
-    <row r="90" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A90" s="1" t="s">
         <v>235</v>
       </c>
@@ -4211,7 +4214,7 @@
         <v>237</v>
       </c>
     </row>
-    <row r="91" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A91" s="1" t="s">
         <v>238</v>
       </c>
@@ -4222,7 +4225,7 @@
         <v>237</v>
       </c>
     </row>
-    <row r="92" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="92" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A92" s="1" t="s">
         <v>240</v>
       </c>
@@ -4233,7 +4236,7 @@
         <v>237</v>
       </c>
     </row>
-    <row r="93" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="93" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A93" s="1" t="s">
         <v>242</v>
       </c>
@@ -4247,7 +4250,7 @@
         <v>244</v>
       </c>
     </row>
-    <row r="94" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="94" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A94" s="1" t="s">
         <v>245</v>
       </c>
@@ -4258,7 +4261,7 @@
         <v>244</v>
       </c>
     </row>
-    <row r="95" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="95" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A95" s="1" t="s">
         <v>247</v>
       </c>
@@ -4272,7 +4275,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="96" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="96" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A96" s="1" t="s">
         <v>251</v>
       </c>
@@ -4283,7 +4286,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="97" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="97" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A97" s="1" t="s">
         <v>253</v>
       </c>
@@ -4294,7 +4297,7 @@
         <v>254</v>
       </c>
     </row>
-    <row r="98" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="98" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A98" s="1" t="s">
         <v>255</v>
       </c>
@@ -4308,7 +4311,7 @@
         <v>258</v>
       </c>
     </row>
-    <row r="99" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="99" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A99" s="1" t="s">
         <v>259</v>
       </c>
@@ -4316,7 +4319,7 @@
         <v>258</v>
       </c>
     </row>
-    <row r="100" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="100" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A100" s="1" t="s">
         <v>260</v>
       </c>
@@ -4324,7 +4327,7 @@
         <v>258</v>
       </c>
     </row>
-    <row r="101" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="101" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A101" s="1" t="s">
         <v>261</v>
       </c>
@@ -4338,7 +4341,7 @@
         <v>263</v>
       </c>
     </row>
-    <row r="102" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="102" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A102" s="1" t="s">
         <v>264</v>
       </c>
@@ -4352,7 +4355,7 @@
         <v>266</v>
       </c>
     </row>
-    <row r="103" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="103" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A103" s="1" t="s">
         <v>267</v>
       </c>
@@ -4366,7 +4369,7 @@
         <v>269</v>
       </c>
     </row>
-    <row r="104" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="104" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A104" s="1" t="s">
         <v>270</v>
       </c>
@@ -4377,7 +4380,7 @@
         <v>269</v>
       </c>
     </row>
-    <row r="105" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="105" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A105" s="1" t="s">
         <v>272</v>
       </c>
@@ -4391,7 +4394,7 @@
         <v>274</v>
       </c>
     </row>
-    <row r="106" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="106" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A106" s="1" t="s">
         <v>275</v>
       </c>
@@ -4405,7 +4408,7 @@
         <v>277</v>
       </c>
     </row>
-    <row r="107" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="107" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A107" s="1" t="s">
         <v>278</v>
       </c>
@@ -4419,7 +4422,7 @@
         <v>280</v>
       </c>
     </row>
-    <row r="108" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="108" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A108" s="1" t="s">
         <v>281</v>
       </c>
@@ -4433,7 +4436,7 @@
         <v>283</v>
       </c>
     </row>
-    <row r="109" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="109" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A109" s="1" t="s">
         <v>284</v>
       </c>
@@ -4447,7 +4450,7 @@
         <v>286</v>
       </c>
     </row>
-    <row r="110" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="110" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A110" s="1" t="s">
         <v>287</v>
       </c>
@@ -4461,7 +4464,7 @@
         <v>289</v>
       </c>
     </row>
-    <row r="111" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="111" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A111" s="1" t="s">
         <v>290</v>
       </c>
@@ -4475,7 +4478,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="112" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="112" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A112" s="1" t="s">
         <v>293</v>
       </c>
@@ -4486,7 +4489,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="113" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="113" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A113" s="1" t="s">
         <v>295</v>
       </c>
@@ -4500,7 +4503,7 @@
         <v>297</v>
       </c>
     </row>
-    <row r="114" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="114" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A114" s="1" t="s">
         <v>298</v>
       </c>
@@ -4511,7 +4514,7 @@
         <v>297</v>
       </c>
     </row>
-    <row r="115" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="115" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A115" s="1" t="s">
         <v>300</v>
       </c>
@@ -4525,7 +4528,7 @@
         <v>302</v>
       </c>
     </row>
-    <row r="116" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="116" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A116" s="1" t="s">
         <v>303</v>
       </c>
@@ -4536,7 +4539,7 @@
         <v>302</v>
       </c>
     </row>
-    <row r="117" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="117" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A117" s="1" t="s">
         <v>305</v>
       </c>
@@ -4547,7 +4550,7 @@
         <v>302</v>
       </c>
     </row>
-    <row r="118" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="118" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A118" s="1" t="s">
         <v>307</v>
       </c>
@@ -4569,7 +4572,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.75" right="0.75" top="0.75" bottom="0.5" header="0.5" footer="0.75"/>
 </worksheet>
@@ -4581,7 +4584,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.75" right="0.75" top="0.75" bottom="0.5" header="0.5" footer="0.75"/>
 </worksheet>
@@ -4593,7 +4596,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.75" right="0.75" top="0.75" bottom="0.5" header="0.5" footer="0.75"/>
 </worksheet>
@@ -4605,7 +4608,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.75" right="0.75" top="0.75" bottom="0.5" header="0.5" footer="0.75"/>
 </worksheet>
@@ -4617,7 +4620,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.75" right="0.75" top="0.75" bottom="0.5" header="0.5" footer="0.75"/>
 </worksheet>
@@ -4629,9 +4632,9 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>617</v>
       </c>
@@ -4654,7 +4657,7 @@
         <v>623</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>624</v>
       </c>
@@ -4674,7 +4677,7 @@
         <v>534</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>625</v>
       </c>
@@ -4694,7 +4697,7 @@
         <v>534</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>625</v>
       </c>
@@ -4714,7 +4717,7 @@
         <v>534</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>625</v>
       </c>
@@ -4734,7 +4737,7 @@
         <v>534</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>626</v>
       </c>
@@ -4765,9 +4768,9 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>549</v>
       </c>
@@ -4793,7 +4796,7 @@
         <v>631</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>632</v>
       </c>
@@ -4819,7 +4822,7 @@
         <v>609</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>635</v>
       </c>
@@ -4845,7 +4848,7 @@
         <v>609</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>637</v>
       </c>
@@ -4882,9 +4885,9 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>514</v>
       </c>
@@ -4910,7 +4913,7 @@
         <v>644</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>637</v>
       </c>
@@ -4921,7 +4924,7 @@
         <v>609</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>637</v>
       </c>
@@ -4935,7 +4938,7 @@
         <v>646</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>637</v>
       </c>
@@ -4946,7 +4949,7 @@
         <v>609</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>637</v>
       </c>
@@ -4957,7 +4960,7 @@
         <v>609</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>637</v>
       </c>
@@ -4968,7 +4971,7 @@
         <v>609</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>637</v>
       </c>
@@ -4979,7 +4982,7 @@
         <v>609</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>637</v>
       </c>
@@ -4990,7 +4993,7 @@
         <v>609</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>637</v>
       </c>
@@ -5001,7 +5004,7 @@
         <v>609</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>637</v>
       </c>
@@ -5012,7 +5015,7 @@
         <v>609</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>632</v>
       </c>
@@ -5023,7 +5026,7 @@
         <v>609</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>632</v>
       </c>
@@ -5034,7 +5037,7 @@
         <v>609</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>635</v>
       </c>
@@ -5056,7 +5059,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.75" right="0.75" top="0.75" bottom="0.5" header="0.5" footer="0.75"/>
 </worksheet>
@@ -5070,76 +5073,76 @@
       <selection activeCell="A13" sqref="A13:A14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="13.33203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="37.6640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="7.6640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.88671875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="13.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="37.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="7.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.85546875" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="17" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="7.5546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="7.5703125" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="7" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="13.5546875" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="13.44140625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="7.5546875" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="11.44140625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="14.33203125" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="12.5546875" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="28.109375" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="14.88671875" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="13.44140625" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="8.33203125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="13.5703125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="13.42578125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="7.5703125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="11.42578125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="14.28515625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="28.140625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="14.85546875" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="13.42578125" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="8.28515625" bestFit="1" customWidth="1"/>
     <col min="18" max="18" width="32" bestFit="1" customWidth="1"/>
     <col min="19" max="19" width="19" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="16.88671875" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="11.44140625" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="30.109375" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="16.85546875" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="11.42578125" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="30.140625" bestFit="1" customWidth="1"/>
     <col min="23" max="23" width="25" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="24.6640625" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="36.88671875" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="20.33203125" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="27.88671875" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="22.33203125" bestFit="1" customWidth="1"/>
-    <col min="29" max="29" width="13.33203125" bestFit="1" customWidth="1"/>
-    <col min="30" max="30" width="16.44140625" bestFit="1" customWidth="1"/>
-    <col min="31" max="31" width="24.5546875" bestFit="1" customWidth="1"/>
-    <col min="32" max="32" width="13.5546875" bestFit="1" customWidth="1"/>
-    <col min="33" max="33" width="9.6640625" bestFit="1" customWidth="1"/>
-    <col min="34" max="34" width="12.109375" bestFit="1" customWidth="1"/>
-    <col min="35" max="35" width="11.5546875" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="24.7109375" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="36.85546875" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="20.28515625" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="27.85546875" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="22.28515625" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="13.28515625" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="16.42578125" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="24.5703125" bestFit="1" customWidth="1"/>
+    <col min="32" max="32" width="13.5703125" bestFit="1" customWidth="1"/>
+    <col min="33" max="33" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="34" max="34" width="12.140625" bestFit="1" customWidth="1"/>
+    <col min="35" max="35" width="11.5703125" bestFit="1" customWidth="1"/>
     <col min="36" max="36" width="29" bestFit="1" customWidth="1"/>
-    <col min="37" max="37" width="28.88671875" bestFit="1" customWidth="1"/>
-    <col min="38" max="38" width="20.5546875" bestFit="1" customWidth="1"/>
-    <col min="39" max="39" width="17.44140625" bestFit="1" customWidth="1"/>
-    <col min="40" max="40" width="26.6640625" bestFit="1" customWidth="1"/>
-    <col min="41" max="41" width="21.44140625" bestFit="1" customWidth="1"/>
-    <col min="42" max="42" width="9.5546875" bestFit="1" customWidth="1"/>
-    <col min="43" max="43" width="27.6640625" bestFit="1" customWidth="1"/>
-    <col min="44" max="44" width="10.109375" bestFit="1" customWidth="1"/>
-    <col min="45" max="45" width="15.109375" bestFit="1" customWidth="1"/>
-    <col min="46" max="46" width="8.44140625" bestFit="1" customWidth="1"/>
-    <col min="47" max="47" width="36.6640625" bestFit="1" customWidth="1"/>
-    <col min="48" max="48" width="14.6640625" bestFit="1" customWidth="1"/>
-    <col min="49" max="49" width="13.5546875" bestFit="1" customWidth="1"/>
-    <col min="50" max="50" width="14.33203125" bestFit="1" customWidth="1"/>
+    <col min="37" max="37" width="28.85546875" bestFit="1" customWidth="1"/>
+    <col min="38" max="38" width="20.5703125" bestFit="1" customWidth="1"/>
+    <col min="39" max="39" width="17.42578125" bestFit="1" customWidth="1"/>
+    <col min="40" max="40" width="26.7109375" bestFit="1" customWidth="1"/>
+    <col min="41" max="41" width="21.42578125" bestFit="1" customWidth="1"/>
+    <col min="42" max="42" width="9.5703125" bestFit="1" customWidth="1"/>
+    <col min="43" max="43" width="27.7109375" bestFit="1" customWidth="1"/>
+    <col min="44" max="44" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="45" max="45" width="15.140625" bestFit="1" customWidth="1"/>
+    <col min="46" max="46" width="8.42578125" bestFit="1" customWidth="1"/>
+    <col min="47" max="47" width="36.7109375" bestFit="1" customWidth="1"/>
+    <col min="48" max="48" width="14.7109375" bestFit="1" customWidth="1"/>
+    <col min="49" max="49" width="13.5703125" bestFit="1" customWidth="1"/>
+    <col min="50" max="50" width="14.28515625" bestFit="1" customWidth="1"/>
     <col min="51" max="51" width="31" bestFit="1" customWidth="1"/>
-    <col min="52" max="52" width="30.44140625" bestFit="1" customWidth="1"/>
-    <col min="53" max="53" width="48.33203125" bestFit="1" customWidth="1"/>
+    <col min="52" max="52" width="30.42578125" bestFit="1" customWidth="1"/>
+    <col min="53" max="53" width="48.28515625" bestFit="1" customWidth="1"/>
     <col min="54" max="54" width="16" bestFit="1" customWidth="1"/>
     <col min="55" max="55" width="21" bestFit="1" customWidth="1"/>
-    <col min="56" max="56" width="15.33203125" bestFit="1" customWidth="1"/>
-    <col min="57" max="57" width="22.109375" bestFit="1" customWidth="1"/>
-    <col min="58" max="59" width="16.33203125" bestFit="1" customWidth="1"/>
-    <col min="60" max="60" width="18.5546875" bestFit="1" customWidth="1"/>
-    <col min="61" max="61" width="24.6640625" bestFit="1" customWidth="1"/>
-    <col min="62" max="62" width="20.88671875" bestFit="1" customWidth="1"/>
-    <col min="63" max="63" width="12.6640625" bestFit="1" customWidth="1"/>
-    <col min="64" max="64" width="15.44140625" bestFit="1" customWidth="1"/>
-    <col min="65" max="65" width="15.33203125" bestFit="1" customWidth="1"/>
+    <col min="56" max="56" width="15.28515625" bestFit="1" customWidth="1"/>
+    <col min="57" max="57" width="22.140625" bestFit="1" customWidth="1"/>
+    <col min="58" max="59" width="16.28515625" bestFit="1" customWidth="1"/>
+    <col min="60" max="60" width="18.5703125" bestFit="1" customWidth="1"/>
+    <col min="61" max="61" width="24.7109375" bestFit="1" customWidth="1"/>
+    <col min="62" max="62" width="20.85546875" bestFit="1" customWidth="1"/>
+    <col min="63" max="63" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="64" max="64" width="15.42578125" bestFit="1" customWidth="1"/>
+    <col min="65" max="65" width="15.28515625" bestFit="1" customWidth="1"/>
     <col min="66" max="66" width="25" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:66" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:66" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>549</v>
       </c>
@@ -5339,7 +5342,7 @@
         <v>699</v>
       </c>
     </row>
-    <row r="2" spans="1:66" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:66" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>700</v>
       </c>
@@ -5383,7 +5386,7 @@
         <v>452</v>
       </c>
     </row>
-    <row r="3" spans="1:66" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:66" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>706</v>
       </c>
@@ -5430,7 +5433,7 @@
         <v>498</v>
       </c>
     </row>
-    <row r="4" spans="1:66" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:66" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>709</v>
       </c>
@@ -5477,7 +5480,7 @@
         <v>498</v>
       </c>
     </row>
-    <row r="5" spans="1:66" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:66" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>711</v>
       </c>
@@ -5524,7 +5527,7 @@
         <v>498</v>
       </c>
     </row>
-    <row r="6" spans="1:66" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:66" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>713</v>
       </c>
@@ -5571,7 +5574,7 @@
         <v>498</v>
       </c>
     </row>
-    <row r="7" spans="1:66" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:66" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>715</v>
       </c>
@@ -5615,7 +5618,7 @@
         <v>452</v>
       </c>
     </row>
-    <row r="8" spans="1:66" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:66" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>717</v>
       </c>
@@ -5659,7 +5662,7 @@
         <v>452</v>
       </c>
     </row>
-    <row r="9" spans="1:66" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:66" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>719</v>
       </c>
@@ -5703,7 +5706,7 @@
         <v>452</v>
       </c>
     </row>
-    <row r="10" spans="1:66" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:66" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>721</v>
       </c>
@@ -5747,7 +5750,7 @@
         <v>452</v>
       </c>
     </row>
-    <row r="11" spans="1:66" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:66" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>849</v>
       </c>
@@ -5791,7 +5794,7 @@
         <v>452</v>
       </c>
     </row>
-    <row r="12" spans="1:66" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:66" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>854</v>
       </c>
@@ -5835,7 +5838,7 @@
         <v>452</v>
       </c>
     </row>
-    <row r="13" spans="1:66" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:66" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>855</v>
       </c>
@@ -5879,7 +5882,7 @@
         <v>452</v>
       </c>
     </row>
-    <row r="14" spans="1:66" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:66" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>856</v>
       </c>
@@ -5935,9 +5938,9 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>309</v>
       </c>
@@ -5951,7 +5954,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>312</v>
       </c>
@@ -5965,7 +5968,7 @@
         <v>315</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>312</v>
       </c>
@@ -5979,7 +5982,7 @@
         <v>318</v>
       </c>
     </row>
-    <row r="4" spans="1:4" ht="388.8" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:4" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>312</v>
       </c>
@@ -5993,7 +5996,7 @@
         <v>321</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>38</v>
       </c>
@@ -6007,7 +6010,7 @@
         <v>324</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>40</v>
       </c>
@@ -6021,7 +6024,7 @@
         <v>324</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>76</v>
       </c>
@@ -6035,7 +6038,7 @@
         <v>328</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>329</v>
       </c>
@@ -6049,7 +6052,7 @@
         <v>332</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>162</v>
       </c>
@@ -6063,7 +6066,7 @@
         <v>335</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>336</v>
       </c>
@@ -6077,7 +6080,7 @@
         <v>339</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>336</v>
       </c>
@@ -6091,7 +6094,7 @@
         <v>342</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>336</v>
       </c>
@@ -6105,7 +6108,7 @@
         <v>345</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>346</v>
       </c>
@@ -6119,7 +6122,7 @@
         <v>349</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
         <v>199</v>
       </c>
@@ -6133,7 +6136,7 @@
         <v>351</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
         <v>352</v>
       </c>
@@ -6147,7 +6150,7 @@
         <v>355</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
         <v>218</v>
       </c>
@@ -6161,7 +6164,7 @@
         <v>358</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
         <v>359</v>
       </c>
@@ -6175,7 +6178,7 @@
         <v>361</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
         <v>359</v>
       </c>
@@ -6189,7 +6192,7 @@
         <v>364</v>
       </c>
     </row>
-    <row r="19" spans="1:4" ht="360" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:4" ht="405" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
         <v>231</v>
       </c>
@@ -6214,7 +6217,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.75" right="0.75" top="0.75" bottom="0.5" header="0.5" footer="0.75"/>
 </worksheet>
@@ -6226,7 +6229,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.75" right="0.75" top="0.75" bottom="0.5" header="0.5" footer="0.75"/>
 </worksheet>
@@ -6238,7 +6241,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.75" right="0.75" top="0.75" bottom="0.5" header="0.5" footer="0.75"/>
 </worksheet>
@@ -6252,7 +6255,7 @@
       <selection activeCell="M28" sqref="M28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.75" right="0.75" top="0.75" bottom="0.5" header="0.5" footer="0.75"/>
 </worksheet>
@@ -6264,7 +6267,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.75" right="0.75" top="0.75" bottom="0.5" header="0.5" footer="0.75"/>
 </worksheet>
@@ -6274,16 +6277,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1800-000000000000}">
   <dimension ref="A1:C12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B10" sqref="A10:B10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="12.44140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>617</v>
       </c>
@@ -6294,7 +6297,7 @@
         <v>723</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>700</v>
       </c>
@@ -6302,7 +6305,7 @@
         <v>706</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>700</v>
       </c>
@@ -6310,7 +6313,7 @@
         <v>709</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>700</v>
       </c>
@@ -6318,7 +6321,7 @@
         <v>711</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>700</v>
       </c>
@@ -6326,7 +6329,7 @@
         <v>713</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>700</v>
       </c>
@@ -6334,7 +6337,7 @@
         <v>715</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>700</v>
       </c>
@@ -6342,7 +6345,7 @@
         <v>717</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>700</v>
       </c>
@@ -6350,7 +6353,7 @@
         <v>719</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>700</v>
       </c>
@@ -6358,7 +6361,7 @@
         <v>721</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>849</v>
       </c>
@@ -6366,7 +6369,7 @@
         <v>854</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>849</v>
       </c>
@@ -6374,7 +6377,7 @@
         <v>855</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>849</v>
       </c>
@@ -6389,13 +6392,20 @@
 
 <file path=xl/worksheets/sheet26.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1900-000000000000}">
-  <dimension ref="A1:C2"/>
+  <dimension ref="A1:C3"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D5" sqref="D5"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="12.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.5703125" customWidth="1"/>
+    <col min="3" max="3" width="9.5703125" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>617</v>
       </c>
@@ -6406,7 +6416,7 @@
         <v>629</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>700</v>
       </c>
@@ -6414,6 +6424,17 @@
         <v>724</v>
       </c>
       <c r="C2" s="1" t="s">
+        <v>534</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>849</v>
+      </c>
+      <c r="B3" t="s">
+        <v>857</v>
+      </c>
+      <c r="C3" t="s">
         <v>534</v>
       </c>
     </row>
@@ -6428,7 +6449,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.75" right="0.75" top="0.75" bottom="0.5" header="0.5" footer="0.75"/>
 </worksheet>
@@ -6440,7 +6461,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.75" right="0.75" top="0.75" bottom="0.5" header="0.5" footer="0.75"/>
 </worksheet>
@@ -6452,7 +6473,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.75" right="0.75" top="0.75" bottom="0.5" header="0.5" footer="0.75"/>
 </worksheet>
@@ -6464,9 +6485,9 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>309</v>
       </c>
@@ -6474,7 +6495,7 @@
         <v>368</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>312</v>
       </c>
@@ -6482,7 +6503,7 @@
         <v>369</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>312</v>
       </c>
@@ -6490,7 +6511,7 @@
         <v>370</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>330</v>
       </c>
@@ -6498,7 +6519,7 @@
         <v>371</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>372</v>
       </c>
@@ -6506,7 +6527,7 @@
         <v>373</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>374</v>
       </c>
@@ -6525,7 +6546,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.75" right="0.75" top="0.75" bottom="0.5" header="0.5" footer="0.75"/>
 </worksheet>
@@ -6537,7 +6558,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.75" right="0.75" top="0.75" bottom="0.5" header="0.5" footer="0.75"/>
 </worksheet>
@@ -6549,7 +6570,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.75" right="0.75" top="0.75" bottom="0.5" header="0.5" footer="0.75"/>
 </worksheet>
@@ -6561,7 +6582,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.75" right="0.75" top="0.75" bottom="0.5" header="0.5" footer="0.75"/>
 </worksheet>
@@ -6573,7 +6594,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.75" right="0.75" top="0.75" bottom="0.5" header="0.5" footer="0.75"/>
 </worksheet>
@@ -6585,7 +6606,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.75" right="0.75" top="0.75" bottom="0.5" header="0.5" footer="0.75"/>
 </worksheet>
@@ -6597,7 +6618,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.75" right="0.75" top="0.75" bottom="0.5" header="0.5" footer="0.75"/>
 </worksheet>
@@ -6609,7 +6630,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.75" right="0.75" top="0.75" bottom="0.5" header="0.5" footer="0.75"/>
 </worksheet>
@@ -6621,7 +6642,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.75" right="0.75" top="0.75" bottom="0.5" header="0.5" footer="0.75"/>
 </worksheet>
@@ -6633,9 +6654,9 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>549</v>
       </c>
@@ -6658,7 +6679,7 @@
         <v>728</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>729</v>
       </c>
@@ -6675,7 +6696,7 @@
         <v>731</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>732</v>
       </c>
@@ -6692,7 +6713,7 @@
         <v>731</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>733</v>
       </c>
@@ -6709,7 +6730,7 @@
         <v>731</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>734</v>
       </c>
@@ -6726,7 +6747,7 @@
         <v>731</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>735</v>
       </c>
@@ -6743,7 +6764,7 @@
         <v>731</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>736</v>
       </c>
@@ -6760,7 +6781,7 @@
         <v>731</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>737</v>
       </c>
@@ -6777,7 +6798,7 @@
         <v>731</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>738</v>
       </c>
@@ -6794,7 +6815,7 @@
         <v>731</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>739</v>
       </c>
@@ -6811,7 +6832,7 @@
         <v>731</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>740</v>
       </c>
@@ -6828,7 +6849,7 @@
         <v>731</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>741</v>
       </c>
@@ -6845,7 +6866,7 @@
         <v>731</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>742</v>
       </c>
@@ -6862,7 +6883,7 @@
         <v>731</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
         <v>743</v>
       </c>
@@ -6890,9 +6911,9 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>375</v>
       </c>
@@ -6900,7 +6921,7 @@
         <v>376</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>377</v>
       </c>
@@ -6908,7 +6929,7 @@
         <v>378</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>293</v>
       </c>
@@ -6916,7 +6937,7 @@
         <v>379</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>140</v>
       </c>
@@ -6924,7 +6945,7 @@
         <v>380</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>142</v>
       </c>
@@ -6943,9 +6964,9 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>744</v>
       </c>
@@ -6989,7 +7010,7 @@
         <v>752</v>
       </c>
     </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>729</v>
       </c>
@@ -7012,7 +7033,7 @@
         <v>754</v>
       </c>
     </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>729</v>
       </c>
@@ -7035,7 +7056,7 @@
         <v>754</v>
       </c>
     </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>729</v>
       </c>
@@ -7058,7 +7079,7 @@
         <v>754</v>
       </c>
     </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>740</v>
       </c>
@@ -7075,7 +7096,7 @@
         <v>754</v>
       </c>
     </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>740</v>
       </c>
@@ -7092,7 +7113,7 @@
         <v>754</v>
       </c>
     </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>740</v>
       </c>
@@ -7109,7 +7130,7 @@
         <v>754</v>
       </c>
     </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>740</v>
       </c>
@@ -7126,7 +7147,7 @@
         <v>754</v>
       </c>
     </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>732</v>
       </c>
@@ -7149,7 +7170,7 @@
         <v>754</v>
       </c>
     </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>732</v>
       </c>
@@ -7172,7 +7193,7 @@
         <v>754</v>
       </c>
     </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>763</v>
       </c>
@@ -7192,7 +7213,7 @@
         <v>754</v>
       </c>
     </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>733</v>
       </c>
@@ -7215,7 +7236,7 @@
         <v>754</v>
       </c>
     </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>733</v>
       </c>
@@ -7238,7 +7259,7 @@
         <v>754</v>
       </c>
     </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
         <v>733</v>
       </c>
@@ -7261,7 +7282,7 @@
         <v>754</v>
       </c>
     </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
         <v>733</v>
       </c>
@@ -7284,7 +7305,7 @@
         <v>754</v>
       </c>
     </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
         <v>733</v>
       </c>
@@ -7307,7 +7328,7 @@
         <v>754</v>
       </c>
     </row>
-    <row r="17" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
         <v>741</v>
       </c>
@@ -7324,7 +7345,7 @@
         <v>754</v>
       </c>
     </row>
-    <row r="18" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
         <v>741</v>
       </c>
@@ -7341,7 +7362,7 @@
         <v>754</v>
       </c>
     </row>
-    <row r="19" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
         <v>741</v>
       </c>
@@ -7358,7 +7379,7 @@
         <v>754</v>
       </c>
     </row>
-    <row r="20" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
         <v>773</v>
       </c>
@@ -7378,7 +7399,7 @@
         <v>754</v>
       </c>
     </row>
-    <row r="21" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
         <v>734</v>
       </c>
@@ -7401,7 +7422,7 @@
         <v>754</v>
       </c>
     </row>
-    <row r="22" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
         <v>742</v>
       </c>
@@ -7418,7 +7439,7 @@
         <v>754</v>
       </c>
     </row>
-    <row r="23" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
         <v>777</v>
       </c>
@@ -7438,7 +7459,7 @@
         <v>754</v>
       </c>
     </row>
-    <row r="24" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
         <v>735</v>
       </c>
@@ -7461,7 +7482,7 @@
         <v>754</v>
       </c>
     </row>
-    <row r="25" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
         <v>735</v>
       </c>
@@ -7484,7 +7505,7 @@
         <v>754</v>
       </c>
     </row>
-    <row r="26" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
         <v>735</v>
       </c>
@@ -7507,7 +7528,7 @@
         <v>754</v>
       </c>
     </row>
-    <row r="27" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
         <v>735</v>
       </c>
@@ -7530,7 +7551,7 @@
         <v>754</v>
       </c>
     </row>
-    <row r="28" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
         <v>735</v>
       </c>
@@ -7553,7 +7574,7 @@
         <v>754</v>
       </c>
     </row>
-    <row r="29" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A29" s="1" t="s">
         <v>743</v>
       </c>
@@ -7570,7 +7591,7 @@
         <v>754</v>
       </c>
     </row>
-    <row r="30" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A30" s="1" t="s">
         <v>785</v>
       </c>
@@ -7590,7 +7611,7 @@
         <v>754</v>
       </c>
     </row>
-    <row r="31" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A31" s="1" t="s">
         <v>736</v>
       </c>
@@ -7613,7 +7634,7 @@
         <v>754</v>
       </c>
     </row>
-    <row r="32" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A32" s="1" t="s">
         <v>736</v>
       </c>
@@ -7636,7 +7657,7 @@
         <v>754</v>
       </c>
     </row>
-    <row r="33" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A33" s="1" t="s">
         <v>736</v>
       </c>
@@ -7659,7 +7680,7 @@
         <v>754</v>
       </c>
     </row>
-    <row r="34" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A34" s="1" t="s">
         <v>736</v>
       </c>
@@ -7682,7 +7703,7 @@
         <v>754</v>
       </c>
     </row>
-    <row r="35" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A35" s="1" t="s">
         <v>736</v>
       </c>
@@ -7705,7 +7726,7 @@
         <v>754</v>
       </c>
     </row>
-    <row r="36" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A36" s="1" t="s">
         <v>737</v>
       </c>
@@ -7728,7 +7749,7 @@
         <v>754</v>
       </c>
     </row>
-    <row r="37" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A37" s="1" t="s">
         <v>737</v>
       </c>
@@ -7751,7 +7772,7 @@
         <v>754</v>
       </c>
     </row>
-    <row r="38" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A38" s="1" t="s">
         <v>738</v>
       </c>
@@ -7774,7 +7795,7 @@
         <v>754</v>
       </c>
     </row>
-    <row r="39" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A39" s="1" t="s">
         <v>738</v>
       </c>
@@ -7797,7 +7818,7 @@
         <v>754</v>
       </c>
     </row>
-    <row r="40" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A40" s="1" t="s">
         <v>738</v>
       </c>
@@ -7820,7 +7841,7 @@
         <v>754</v>
       </c>
     </row>
-    <row r="41" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A41" s="1" t="s">
         <v>738</v>
       </c>
@@ -7843,7 +7864,7 @@
         <v>754</v>
       </c>
     </row>
-    <row r="42" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A42" s="1" t="s">
         <v>739</v>
       </c>
@@ -7866,7 +7887,7 @@
         <v>754</v>
       </c>
     </row>
-    <row r="43" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A43" s="1" t="s">
         <v>739</v>
       </c>
@@ -7889,7 +7910,7 @@
         <v>754</v>
       </c>
     </row>
-    <row r="44" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A44" s="1" t="s">
         <v>739</v>
       </c>
@@ -7912,7 +7933,7 @@
         <v>754</v>
       </c>
     </row>
-    <row r="45" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A45" s="1" t="s">
         <v>739</v>
       </c>
@@ -7946,7 +7967,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.75" right="0.75" top="0.75" bottom="0.5" header="0.5" footer="0.75"/>
 </worksheet>
@@ -7958,7 +7979,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.75" right="0.75" top="0.75" bottom="0.5" header="0.5" footer="0.75"/>
 </worksheet>
@@ -7970,9 +7991,9 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>549</v>
       </c>
@@ -8019,7 +8040,7 @@
         <v>811</v>
       </c>
     </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>812</v>
       </c>
@@ -8063,7 +8084,7 @@
         <v>609</v>
       </c>
     </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>814</v>
       </c>
@@ -8118,9 +8139,9 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>816</v>
       </c>
@@ -8158,7 +8179,7 @@
         <v>824</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>812</v>
       </c>
@@ -8190,7 +8211,7 @@
         <v>450</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>812</v>
       </c>
@@ -8222,7 +8243,7 @@
         <v>449</v>
       </c>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>812</v>
       </c>
@@ -8254,7 +8275,7 @@
         <v>827</v>
       </c>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>812</v>
       </c>
@@ -8289,7 +8310,7 @@
         <v>829</v>
       </c>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>812</v>
       </c>
@@ -8324,7 +8345,7 @@
         <v>450</v>
       </c>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>812</v>
       </c>
@@ -8359,7 +8380,7 @@
         <v>450</v>
       </c>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>812</v>
       </c>
@@ -8391,7 +8412,7 @@
         <v>450</v>
       </c>
     </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>812</v>
       </c>
@@ -8423,7 +8444,7 @@
         <v>450</v>
       </c>
     </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>812</v>
       </c>
@@ -8455,7 +8476,7 @@
         <v>450</v>
       </c>
     </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>814</v>
       </c>
@@ -8487,7 +8508,7 @@
         <v>450</v>
       </c>
     </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>814</v>
       </c>
@@ -8519,7 +8540,7 @@
         <v>827</v>
       </c>
     </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>814</v>
       </c>
@@ -8551,7 +8572,7 @@
         <v>829</v>
       </c>
     </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
         <v>814</v>
       </c>
@@ -8594,9 +8615,9 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>549</v>
       </c>
@@ -8610,7 +8631,7 @@
         <v>832</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>813</v>
       </c>
@@ -8621,7 +8642,7 @@
         <v>834</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>815</v>
       </c>
@@ -8643,9 +8664,9 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>802</v>
       </c>
@@ -8668,7 +8689,7 @@
         <v>319</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>813</v>
       </c>
@@ -8685,7 +8706,7 @@
         <v>609</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>813</v>
       </c>
@@ -8702,7 +8723,7 @@
         <v>609</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>813</v>
       </c>
@@ -8719,7 +8740,7 @@
         <v>609</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>813</v>
       </c>
@@ -8736,7 +8757,7 @@
         <v>609</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>813</v>
       </c>
@@ -8753,7 +8774,7 @@
         <v>609</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>813</v>
       </c>
@@ -8770,7 +8791,7 @@
         <v>609</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>813</v>
       </c>
@@ -8787,7 +8808,7 @@
         <v>609</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>813</v>
       </c>
@@ -8804,7 +8825,7 @@
         <v>609</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>813</v>
       </c>
@@ -8821,7 +8842,7 @@
         <v>534</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>815</v>
       </c>
@@ -8838,7 +8859,7 @@
         <v>609</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>815</v>
       </c>
@@ -8855,7 +8876,7 @@
         <v>609</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>815</v>
       </c>
@@ -8872,7 +8893,7 @@
         <v>609</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
         <v>815</v>
       </c>
@@ -8900,9 +8921,9 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>802</v>
       </c>
@@ -8928,7 +8949,7 @@
         <v>840</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>813</v>
       </c>
@@ -8945,7 +8966,7 @@
         <v>732</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>813</v>
       </c>
@@ -8962,7 +8983,7 @@
         <v>733</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>813</v>
       </c>
@@ -8979,7 +9000,7 @@
         <v>734</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>813</v>
       </c>
@@ -8996,7 +9017,7 @@
         <v>735</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>813</v>
       </c>
@@ -9013,7 +9034,7 @@
         <v>736</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>813</v>
       </c>
@@ -9030,7 +9051,7 @@
         <v>737</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>813</v>
       </c>
@@ -9047,7 +9068,7 @@
         <v>738</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>813</v>
       </c>
@@ -9064,7 +9085,7 @@
         <v>739</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>815</v>
       </c>
@@ -9081,7 +9102,7 @@
         <v>741</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>815</v>
       </c>
@@ -9098,7 +9119,7 @@
         <v>742</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>815</v>
       </c>
@@ -9126,814 +9147,814 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>382</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>383</v>
       </c>
     </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>384</v>
       </c>
     </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>385</v>
       </c>
     </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>386</v>
       </c>
     </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>387</v>
       </c>
     </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>388</v>
       </c>
     </row>
-    <row r="8" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>389</v>
       </c>
     </row>
-    <row r="9" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>390</v>
       </c>
     </row>
-    <row r="10" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>391</v>
       </c>
     </row>
-    <row r="11" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>392</v>
       </c>
     </row>
-    <row r="12" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>393</v>
       </c>
     </row>
-    <row r="14" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>394</v>
       </c>
     </row>
-    <row r="15" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
         <v>395</v>
       </c>
     </row>
-    <row r="16" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
         <v>396</v>
       </c>
     </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
         <v>397</v>
       </c>
     </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>398</v>
       </c>
     </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
         <v>399</v>
       </c>
     </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
         <v>400</v>
       </c>
     </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>401</v>
       </c>
     </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
         <v>402</v>
       </c>
     </row>
-    <row r="25" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
         <v>403</v>
       </c>
     </row>
-    <row r="26" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
         <v>404</v>
       </c>
     </row>
-    <row r="27" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
         <v>405</v>
       </c>
     </row>
-    <row r="29" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>406</v>
       </c>
     </row>
-    <row r="30" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A30" s="1" t="s">
         <v>407</v>
       </c>
     </row>
-    <row r="31" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A31" s="1" t="s">
         <v>408</v>
       </c>
     </row>
-    <row r="32" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A32" s="1" t="s">
         <v>409</v>
       </c>
     </row>
-    <row r="34" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>410</v>
       </c>
     </row>
-    <row r="35" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A35" s="1" t="s">
         <v>411</v>
       </c>
     </row>
-    <row r="36" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A36" s="1" t="s">
         <v>412</v>
       </c>
     </row>
-    <row r="37" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A37" s="1" t="s">
         <v>413</v>
       </c>
     </row>
-    <row r="38" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A38" s="1" t="s">
         <v>414</v>
       </c>
     </row>
-    <row r="39" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A39" s="1" t="s">
         <v>415</v>
       </c>
     </row>
-    <row r="40" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A40" s="1" t="s">
         <v>416</v>
       </c>
     </row>
-    <row r="41" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A41" s="1" t="s">
         <v>417</v>
       </c>
     </row>
-    <row r="42" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A42" s="1" t="s">
         <v>418</v>
       </c>
     </row>
-    <row r="44" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>419</v>
       </c>
     </row>
-    <row r="45" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A45" s="1" t="s">
         <v>420</v>
       </c>
     </row>
-    <row r="46" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A46" s="1" t="s">
         <v>421</v>
       </c>
     </row>
-    <row r="47" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A47" s="1" t="s">
         <v>422</v>
       </c>
     </row>
-    <row r="48" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A48" s="1" t="s">
         <v>423</v>
       </c>
     </row>
-    <row r="50" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>424</v>
       </c>
     </row>
-    <row r="51" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A51" s="1" t="s">
         <v>425</v>
       </c>
     </row>
-    <row r="52" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A52" s="1" t="s">
         <v>426</v>
       </c>
     </row>
-    <row r="54" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
         <v>427</v>
       </c>
     </row>
-    <row r="55" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A55" s="1" t="s">
         <v>428</v>
       </c>
     </row>
-    <row r="56" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A56" s="1" t="s">
         <v>429</v>
       </c>
     </row>
-    <row r="57" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A57" s="1" t="s">
         <v>430</v>
       </c>
     </row>
-    <row r="58" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A58" s="1" t="s">
         <v>431</v>
       </c>
     </row>
-    <row r="59" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A59" s="1" t="s">
         <v>432</v>
       </c>
     </row>
-    <row r="60" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A60" s="1" t="s">
         <v>433</v>
       </c>
     </row>
-    <row r="61" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A61" s="1" t="s">
         <v>434</v>
       </c>
     </row>
-    <row r="62" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A62" s="1" t="s">
         <v>435</v>
       </c>
     </row>
-    <row r="64" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
         <v>436</v>
       </c>
     </row>
-    <row r="65" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A65" s="1" t="s">
         <v>437</v>
       </c>
     </row>
-    <row r="66" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A66" s="1" t="s">
         <v>438</v>
       </c>
     </row>
-    <row r="68" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
         <v>439</v>
       </c>
     </row>
-    <row r="69" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A69" s="1" t="s">
         <v>440</v>
       </c>
     </row>
-    <row r="70" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A70" s="1" t="s">
         <v>441</v>
       </c>
     </row>
-    <row r="71" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A71" s="1" t="s">
         <v>442</v>
       </c>
     </row>
-    <row r="73" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
         <v>443</v>
       </c>
     </row>
-    <row r="74" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A74" s="1" t="s">
         <v>444</v>
       </c>
     </row>
-    <row r="75" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A75" s="1" t="s">
         <v>445</v>
       </c>
     </row>
-    <row r="76" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A76" s="1" t="s">
         <v>446</v>
       </c>
     </row>
-    <row r="77" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A77" s="1" t="s">
         <v>447</v>
       </c>
     </row>
-    <row r="79" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
         <v>448</v>
       </c>
     </row>
-    <row r="80" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A80" s="1" t="s">
         <v>449</v>
       </c>
     </row>
-    <row r="81" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A81" s="1" t="s">
         <v>450</v>
       </c>
     </row>
-    <row r="83" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
         <v>451</v>
       </c>
     </row>
-    <row r="84" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A84" s="1" t="s">
         <v>450</v>
       </c>
     </row>
-    <row r="85" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A85" s="1" t="s">
         <v>452</v>
       </c>
     </row>
-    <row r="86" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A86" s="1" t="s">
         <v>403</v>
       </c>
     </row>
-    <row r="88" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
         <v>453</v>
       </c>
     </row>
-    <row r="89" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A89" s="1" t="s">
         <v>454</v>
       </c>
     </row>
-    <row r="90" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A90" s="1" t="s">
         <v>455</v>
       </c>
     </row>
-    <row r="92" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="92" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
         <v>456</v>
       </c>
     </row>
-    <row r="93" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="93" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A93" s="1" t="s">
         <v>457</v>
       </c>
     </row>
-    <row r="94" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="94" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A94" s="1" t="s">
         <v>458</v>
       </c>
     </row>
-    <row r="96" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="96" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
         <v>459</v>
       </c>
     </row>
-    <row r="97" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="97" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A97" s="1" t="s">
         <v>460</v>
       </c>
     </row>
-    <row r="98" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="98" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A98" s="1" t="s">
         <v>461</v>
       </c>
     </row>
-    <row r="100" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="100" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
         <v>462</v>
       </c>
     </row>
-    <row r="101" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="101" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A101" s="1" t="s">
         <v>463</v>
       </c>
     </row>
-    <row r="102" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="102" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A102" s="1" t="s">
         <v>464</v>
       </c>
     </row>
-    <row r="103" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="103" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A103" s="1" t="s">
         <v>465</v>
       </c>
     </row>
-    <row r="104" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="104" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A104" s="1" t="s">
         <v>466</v>
       </c>
     </row>
-    <row r="106" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="106" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A106" t="s">
         <v>467</v>
       </c>
     </row>
-    <row r="107" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="107" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A107" s="1" t="s">
         <v>468</v>
       </c>
     </row>
-    <row r="108" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="108" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A108" s="1" t="s">
         <v>469</v>
       </c>
     </row>
-    <row r="109" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="109" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A109" s="1" t="s">
         <v>470</v>
       </c>
     </row>
-    <row r="110" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="110" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A110" s="1" t="s">
         <v>471</v>
       </c>
     </row>
-    <row r="111" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="111" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A111" s="1" t="s">
         <v>472</v>
       </c>
     </row>
-    <row r="112" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="112" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A112" s="1" t="s">
         <v>473</v>
       </c>
     </row>
-    <row r="114" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="114" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A114" t="s">
         <v>474</v>
       </c>
     </row>
-    <row r="115" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="115" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A115" s="1" t="s">
         <v>475</v>
       </c>
     </row>
-    <row r="116" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="116" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A116" s="1" t="s">
         <v>476</v>
       </c>
     </row>
-    <row r="118" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="118" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A118" t="s">
         <v>477</v>
       </c>
     </row>
-    <row r="119" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="119" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A119" s="1" t="s">
         <v>464</v>
       </c>
     </row>
-    <row r="120" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="120" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A120" s="1" t="s">
         <v>463</v>
       </c>
     </row>
-    <row r="121" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="121" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A121" s="1" t="s">
         <v>478</v>
       </c>
     </row>
-    <row r="122" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="122" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A122" s="1" t="s">
         <v>479</v>
       </c>
     </row>
-    <row r="123" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="123" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A123" s="1" t="s">
         <v>480</v>
       </c>
     </row>
-    <row r="125" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="125" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A125" t="s">
         <v>481</v>
       </c>
     </row>
-    <row r="126" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="126" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A126" s="1" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="127" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="127" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A127" s="1" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="128" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="128" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A128" s="1" t="s">
         <v>482</v>
       </c>
     </row>
-    <row r="129" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="129" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A129" s="1" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="130" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="130" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A130" s="1" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="131" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="131" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A131" s="1" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="132" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="132" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A132" s="1" t="s">
         <v>483</v>
       </c>
     </row>
-    <row r="133" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="133" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A133" s="1" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="135" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="135" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A135" t="s">
         <v>484</v>
       </c>
     </row>
-    <row r="136" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="136" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A136" s="1" t="s">
         <v>485</v>
       </c>
     </row>
-    <row r="137" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="137" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A137" s="1" t="s">
         <v>486</v>
       </c>
     </row>
-    <row r="139" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="139" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A139" t="s">
         <v>487</v>
       </c>
     </row>
-    <row r="140" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="140" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A140" s="1" t="s">
         <v>488</v>
       </c>
     </row>
-    <row r="141" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="141" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A141" s="1" t="s">
         <v>489</v>
       </c>
     </row>
-    <row r="143" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="143" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A143" t="s">
         <v>490</v>
       </c>
     </row>
-    <row r="144" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="144" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A144" s="1" t="s">
         <v>491</v>
       </c>
     </row>
-    <row r="145" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="145" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A145" s="1" t="s">
         <v>449</v>
       </c>
     </row>
-    <row r="147" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="147" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A147" t="s">
         <v>492</v>
       </c>
     </row>
-    <row r="148" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="148" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A148" s="1" t="s">
         <v>493</v>
       </c>
     </row>
-    <row r="149" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="149" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A149" s="1" t="s">
         <v>494</v>
       </c>
     </row>
-    <row r="150" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="150" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A150" s="1" t="s">
         <v>495</v>
       </c>
     </row>
-    <row r="152" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="152" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A152" t="s">
         <v>496</v>
       </c>
     </row>
-    <row r="153" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="153" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A153" s="1" t="s">
         <v>497</v>
       </c>
     </row>
-    <row r="154" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="154" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A154" s="1" t="s">
         <v>498</v>
       </c>
     </row>
-    <row r="156" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="156" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A156" t="s">
         <v>499</v>
       </c>
     </row>
-    <row r="157" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="157" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A157" s="1" t="s">
         <v>500</v>
       </c>
     </row>
-    <row r="158" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="158" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A158" s="1" t="s">
         <v>501</v>
       </c>
     </row>
-    <row r="159" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="159" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A159" s="1" t="s">
         <v>502</v>
       </c>
     </row>
-    <row r="161" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="161" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A161" t="s">
         <v>503</v>
       </c>
     </row>
-    <row r="162" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="162" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A162" s="1" t="s">
         <v>504</v>
       </c>
     </row>
-    <row r="163" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="163" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A163" s="1" t="s">
         <v>505</v>
       </c>
     </row>
-    <row r="165" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="165" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A165" t="s">
         <v>506</v>
       </c>
     </row>
-    <row r="166" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="166" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A166" s="1" t="s">
         <v>507</v>
       </c>
     </row>
-    <row r="167" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="167" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A167" s="1" t="s">
         <v>508</v>
       </c>
     </row>
-    <row r="168" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="168" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A168" s="1" t="s">
         <v>509</v>
       </c>
     </row>
-    <row r="169" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="169" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A169" s="1" t="s">
         <v>510</v>
       </c>
     </row>
-    <row r="170" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="170" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A170" s="1" t="s">
         <v>415</v>
       </c>
     </row>
-    <row r="172" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="172" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A172" t="s">
         <v>511</v>
       </c>
     </row>
-    <row r="173" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="173" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A173" s="1" t="s">
         <v>468</v>
       </c>
     </row>
-    <row r="174" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="174" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A174" s="1" t="s">
         <v>403</v>
       </c>
     </row>
-    <row r="175" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="175" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A175" s="1" t="s">
         <v>404</v>
       </c>
     </row>
-    <row r="176" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="176" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A176" s="1" t="s">
         <v>497</v>
       </c>
     </row>
-    <row r="177" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="177" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A177" s="1" t="s">
         <v>512</v>
       </c>
     </row>
-    <row r="178" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="178" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A178" s="1" t="s">
         <v>513</v>
       </c>
     </row>
-    <row r="179" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="179" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A179" s="1" t="s">
         <v>514</v>
       </c>
     </row>
-    <row r="181" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="181" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A181" t="s">
         <v>515</v>
       </c>
     </row>
-    <row r="182" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="182" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A182" s="1" t="s">
         <v>516</v>
       </c>
     </row>
-    <row r="183" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="183" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A183" s="1" t="s">
         <v>517</v>
       </c>
     </row>
-    <row r="184" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="184" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A184" s="1" t="s">
         <v>518</v>
       </c>
     </row>
-    <row r="185" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="185" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A185" s="1" t="s">
         <v>519</v>
       </c>
     </row>
-    <row r="186" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="186" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A186" s="1" t="s">
         <v>520</v>
       </c>
     </row>
-    <row r="187" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="187" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A187" s="1" t="s">
         <v>521</v>
       </c>
     </row>
-    <row r="188" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="188" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A188" s="1" t="s">
         <v>522</v>
       </c>
     </row>
-    <row r="189" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="189" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A189" s="1" t="s">
         <v>523</v>
       </c>
     </row>
-    <row r="190" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="190" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A190" s="1" t="s">
         <v>485</v>
       </c>
     </row>
-    <row r="191" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="191" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A191" s="1" t="s">
         <v>524</v>
       </c>
     </row>
-    <row r="192" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="192" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A192" s="1" t="s">
         <v>525</v>
       </c>
     </row>
-    <row r="193" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="193" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A193" s="1" t="s">
         <v>526</v>
       </c>
@@ -9949,9 +9970,9 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>527</v>
       </c>
@@ -9968,7 +9989,7 @@
         <v>531</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>532</v>
       </c>
@@ -9982,7 +10003,7 @@
         <v>534</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>532</v>
       </c>
@@ -9996,7 +10017,7 @@
         <v>534</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>532</v>
       </c>
@@ -10010,7 +10031,7 @@
         <v>534</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>532</v>
       </c>
@@ -10024,7 +10045,7 @@
         <v>534</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>532</v>
       </c>
@@ -10038,7 +10059,7 @@
         <v>534</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>532</v>
       </c>
@@ -10052,7 +10073,7 @@
         <v>534</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>540</v>
       </c>
@@ -10066,7 +10087,7 @@
         <v>534</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>542</v>
       </c>
@@ -10080,7 +10101,7 @@
         <v>534</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>542</v>
       </c>
@@ -10094,7 +10115,7 @@
         <v>534</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>542</v>
       </c>
@@ -10108,7 +10129,7 @@
         <v>534</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>542</v>
       </c>
@@ -10122,7 +10143,7 @@
         <v>534</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>542</v>
       </c>
@@ -10136,7 +10157,7 @@
         <v>534</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
         <v>542</v>
       </c>
@@ -10150,7 +10171,7 @@
         <v>534</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
         <v>547</v>
       </c>
@@ -10175,9 +10196,9 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>549</v>
       </c>
@@ -10194,7 +10215,7 @@
         <v>552</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>553</v>
       </c>
@@ -10205,7 +10226,7 @@
         <v>555</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>556</v>
       </c>
@@ -10216,7 +10237,7 @@
         <v>555</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>557</v>
       </c>
@@ -10227,7 +10248,7 @@
         <v>555</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>558</v>
       </c>
@@ -10238,7 +10259,7 @@
         <v>555</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>560</v>
       </c>
@@ -10260,9 +10281,9 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:47" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>549</v>
       </c>
@@ -10405,7 +10426,7 @@
         <v>604</v>
       </c>
     </row>
-    <row r="2" spans="1:47" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>605</v>
       </c>
@@ -10449,7 +10470,7 @@
         <v>611</v>
       </c>
     </row>
-    <row r="3" spans="1:47" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>612</v>
       </c>
@@ -10504,7 +10525,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.75" right="0.75" top="0.75" bottom="0.5" header="0.5" footer="0.75"/>
 </worksheet>

</xml_diff>